<commit_message>
Imported Tuning as option in settings
</commit_message>
<xml_diff>
--- a/RECOVER/assets/texts/texts.xlsx
+++ b/RECOVER/assets/texts/texts.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1373825" uniqueCount="1937">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1389038" uniqueCount="1946">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -6951,6 +6951,33 @@
   </si>
   <si>
     <t xml:space="preserve">SingleUseId250</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Widget Wildcard Characters</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId251</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Start Tuning Cycle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Tuning</t>
+  </si>
+  <si>
+    <t xml:space="preserve">调音</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Réglage</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sintonización</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Messa a punto</t>
+  </si>
+  <si>
+    <t xml:space="preserve">настройка</t>
   </si>
 </sst>
 </file>
@@ -8158,6 +8185,9 @@
       <c r="I3" s="20" t="s">
         <v>28</v>
       </c>
+      <c r="J3" t="s">
+        <v>1937</v>
+      </c>
     </row>
     <row r="4" spans="2:15">
       <c r="B4" t="s">
@@ -8182,6 +8212,7 @@
         <v>78</v>
       </c>
       <c r="I4"/>
+      <c r="J4"/>
       <c r="K4" s="4" t="s">
         <v>9</v>
       </c>
@@ -8221,6 +8252,7 @@
         <v>78</v>
       </c>
       <c r="I5"/>
+      <c r="J5"/>
       <c r="K5" s="7" t="s">
         <v>1</v>
       </c>
@@ -8256,6 +8288,7 @@
         <v>78</v>
       </c>
       <c r="I6"/>
+      <c r="J6"/>
       <c r="K6" s="7" t="s">
         <v>2</v>
       </c>
@@ -8291,6 +8324,7 @@
       </c>
       <c r="H7"/>
       <c r="I7"/>
+      <c r="J7"/>
       <c r="K7" s="7" t="s">
         <v>7</v>
       </c>
@@ -8330,6 +8364,7 @@
         <v>78</v>
       </c>
       <c r="I8"/>
+      <c r="J8"/>
       <c r="K8" s="7" t="s">
         <v>8</v>
       </c>
@@ -8363,6 +8398,7 @@
       <c r="G9"/>
       <c r="H9"/>
       <c r="I9"/>
+      <c r="J9"/>
       <c r="K9" s="11" t="s">
         <v>6</v>
       </c>
@@ -8400,6 +8436,7 @@
         <v>78</v>
       </c>
       <c r="I10"/>
+      <c r="J10"/>
       <c r="K10" s="11" t="s">
         <v>28</v>
       </c>
@@ -8435,6 +8472,7 @@
         <v>78</v>
       </c>
       <c r="I11"/>
+      <c r="J11"/>
       <c r="K11" s="15"/>
     </row>
     <row r="12" spans="2:15">
@@ -8458,6 +8496,7 @@
         <v>78</v>
       </c>
       <c r="I12"/>
+      <c r="J12"/>
       <c r="L12" s="16" t="s">
         <v>27</v>
       </c>
@@ -8485,6 +8524,7 @@
         <v>78</v>
       </c>
       <c r="I13"/>
+      <c r="J13"/>
     </row>
     <row r="14" spans="2:15">
       <c r="B14" t="s">
@@ -8509,6 +8549,7 @@
         <v>78</v>
       </c>
       <c r="I14"/>
+      <c r="J14"/>
     </row>
     <row r="15" spans="2:15">
       <c r="B15" t="s">
@@ -8529,6 +8570,7 @@
       <c r="G15"/>
       <c r="H15"/>
       <c r="I15"/>
+      <c r="J15"/>
     </row>
     <row r="16" spans="2:15">
       <c r="B16" t="s">
@@ -8553,6 +8595,7 @@
         <v>78</v>
       </c>
       <c r="I16"/>
+      <c r="J16"/>
     </row>
   </sheetData>
   <sheetProtection sheet="0" objects="0" scenarios="0" formatCells="0" formatColumns="0" formatRows="0" insertColumns="0" insertRows="0" insertHyperlinks="0" deleteColumns="0" deleteRows="0" selectLockedCells="1" sort="0" autoFilter="0" pivotTables="0" selectUnlockedCells="1"/>
@@ -17250,7 +17293,7 @@
     </row>
     <row r="219">
       <c r="B219" t="s">
-        <v>1831</v>
+        <v>1834</v>
       </c>
       <c r="C219" t="s">
         <v>39</v>
@@ -17262,77 +17305,74 @@
         <v>41</v>
       </c>
       <c r="F219" t="s">
-        <v>1833</v>
+        <v>1888</v>
       </c>
       <c r="G219" t="s">
-        <v>1836</v>
+        <v>1847</v>
       </c>
       <c r="H219" t="s">
-        <v>131</v>
+        <v>134</v>
       </c>
       <c r="I219" t="s">
-        <v>1837</v>
+        <v>1848</v>
       </c>
       <c r="J219" t="s">
-        <v>1838</v>
+        <v>1849</v>
       </c>
       <c r="K219" t="s">
-        <v>1839</v>
+        <v>1843</v>
       </c>
       <c r="L219" t="s">
-        <v>1840</v>
+        <v>1844</v>
       </c>
       <c r="M219" t="s">
-        <v>1841</v>
+        <v>1845</v>
       </c>
       <c r="N219" t="s">
-        <v>1842</v>
+        <v>1846</v>
       </c>
     </row>
     <row r="220">
       <c r="B220" t="s">
-        <v>1834</v>
+        <v>1856</v>
       </c>
       <c r="C220" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="D220" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E220" t="s">
         <v>41</v>
       </c>
       <c r="F220" t="s">
-        <v>1888</v>
+        <v>1853</v>
       </c>
       <c r="G220" t="s">
-        <v>1847</v>
-      </c>
-      <c r="H220" t="s">
-        <v>134</v>
+        <v>1047</v>
       </c>
       <c r="I220" t="s">
-        <v>1848</v>
+        <v>1047</v>
       </c>
       <c r="J220" t="s">
-        <v>1849</v>
+        <v>1047</v>
       </c>
       <c r="K220" t="s">
-        <v>1843</v>
+        <v>1047</v>
       </c>
       <c r="L220" t="s">
-        <v>1844</v>
+        <v>1047</v>
       </c>
       <c r="M220" t="s">
-        <v>1845</v>
+        <v>1047</v>
       </c>
       <c r="N220" t="s">
-        <v>1846</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="221">
       <c r="B221" t="s">
-        <v>1856</v>
+        <v>1857</v>
       </c>
       <c r="C221" t="s">
         <v>38</v>
@@ -17344,7 +17384,7 @@
         <v>41</v>
       </c>
       <c r="F221" t="s">
-        <v>1853</v>
+        <v>1873</v>
       </c>
       <c r="G221" t="s">
         <v>1047</v>
@@ -17370,7 +17410,7 @@
     </row>
     <row r="222">
       <c r="B222" t="s">
-        <v>1857</v>
+        <v>1858</v>
       </c>
       <c r="C222" t="s">
         <v>38</v>
@@ -17382,7 +17422,7 @@
         <v>41</v>
       </c>
       <c r="F222" t="s">
-        <v>1873</v>
+        <v>1874</v>
       </c>
       <c r="G222" t="s">
         <v>1047</v>
@@ -17408,7 +17448,7 @@
     </row>
     <row r="223">
       <c r="B223" t="s">
-        <v>1858</v>
+        <v>1859</v>
       </c>
       <c r="C223" t="s">
         <v>38</v>
@@ -17420,7 +17460,7 @@
         <v>41</v>
       </c>
       <c r="F223" t="s">
-        <v>1874</v>
+        <v>936</v>
       </c>
       <c r="G223" t="s">
         <v>1047</v>
@@ -17446,7 +17486,7 @@
     </row>
     <row r="224">
       <c r="B224" t="s">
-        <v>1859</v>
+        <v>1861</v>
       </c>
       <c r="C224" t="s">
         <v>38</v>
@@ -17458,7 +17498,7 @@
         <v>41</v>
       </c>
       <c r="F224" t="s">
-        <v>936</v>
+        <v>1885</v>
       </c>
       <c r="G224" t="s">
         <v>1047</v>
@@ -17484,7 +17524,7 @@
     </row>
     <row r="225">
       <c r="B225" t="s">
-        <v>1861</v>
+        <v>1862</v>
       </c>
       <c r="C225" t="s">
         <v>38</v>
@@ -17496,7 +17536,7 @@
         <v>41</v>
       </c>
       <c r="F225" t="s">
-        <v>1885</v>
+        <v>1869</v>
       </c>
       <c r="G225" t="s">
         <v>1047</v>
@@ -17522,7 +17562,7 @@
     </row>
     <row r="226">
       <c r="B226" t="s">
-        <v>1862</v>
+        <v>1863</v>
       </c>
       <c r="C226" t="s">
         <v>38</v>
@@ -17534,7 +17574,7 @@
         <v>41</v>
       </c>
       <c r="F226" t="s">
-        <v>1869</v>
+        <v>1875</v>
       </c>
       <c r="G226" t="s">
         <v>1047</v>
@@ -17560,7 +17600,7 @@
     </row>
     <row r="227">
       <c r="B227" t="s">
-        <v>1863</v>
+        <v>1864</v>
       </c>
       <c r="C227" t="s">
         <v>38</v>
@@ -17572,7 +17612,7 @@
         <v>41</v>
       </c>
       <c r="F227" t="s">
-        <v>1875</v>
+        <v>1876</v>
       </c>
       <c r="G227" t="s">
         <v>1047</v>
@@ -17598,7 +17638,7 @@
     </row>
     <row r="228">
       <c r="B228" t="s">
-        <v>1864</v>
+        <v>1865</v>
       </c>
       <c r="C228" t="s">
         <v>38</v>
@@ -17610,7 +17650,7 @@
         <v>41</v>
       </c>
       <c r="F228" t="s">
-        <v>1876</v>
+        <v>1870</v>
       </c>
       <c r="G228" t="s">
         <v>1047</v>
@@ -17636,7 +17676,7 @@
     </row>
     <row r="229">
       <c r="B229" t="s">
-        <v>1865</v>
+        <v>1866</v>
       </c>
       <c r="C229" t="s">
         <v>38</v>
@@ -17648,7 +17688,7 @@
         <v>41</v>
       </c>
       <c r="F229" t="s">
-        <v>1870</v>
+        <v>1877</v>
       </c>
       <c r="G229" t="s">
         <v>1047</v>
@@ -17674,7 +17714,7 @@
     </row>
     <row r="230">
       <c r="B230" t="s">
-        <v>1866</v>
+        <v>1867</v>
       </c>
       <c r="C230" t="s">
         <v>38</v>
@@ -17686,7 +17726,7 @@
         <v>41</v>
       </c>
       <c r="F230" t="s">
-        <v>1877</v>
+        <v>1878</v>
       </c>
       <c r="G230" t="s">
         <v>1047</v>
@@ -17712,7 +17752,7 @@
     </row>
     <row r="231">
       <c r="B231" t="s">
-        <v>1867</v>
+        <v>1879</v>
       </c>
       <c r="C231" t="s">
         <v>38</v>
@@ -17724,7 +17764,7 @@
         <v>41</v>
       </c>
       <c r="F231" t="s">
-        <v>1878</v>
+        <v>1887</v>
       </c>
       <c r="G231" t="s">
         <v>1047</v>
@@ -17750,10 +17790,10 @@
     </row>
     <row r="232">
       <c r="B232" t="s">
-        <v>1879</v>
+        <v>1881</v>
       </c>
       <c r="C232" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D232" t="s">
         <v>40</v>
@@ -17762,7 +17802,7 @@
         <v>41</v>
       </c>
       <c r="F232" t="s">
-        <v>1887</v>
+        <v>1882</v>
       </c>
       <c r="G232" t="s">
         <v>1047</v>
@@ -17788,10 +17828,10 @@
     </row>
     <row r="233">
       <c r="B233" t="s">
-        <v>1881</v>
+        <v>1883</v>
       </c>
       <c r="C233" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="D233" t="s">
         <v>40</v>
@@ -17800,36 +17840,36 @@
         <v>41</v>
       </c>
       <c r="F233" t="s">
-        <v>1882</v>
+        <v>43</v>
       </c>
       <c r="G233" t="s">
-        <v>1047</v>
+        <v>43</v>
       </c>
       <c r="I233" t="s">
-        <v>1047</v>
+        <v>43</v>
       </c>
       <c r="J233" t="s">
-        <v>1047</v>
+        <v>43</v>
       </c>
       <c r="K233" t="s">
-        <v>1047</v>
+        <v>43</v>
       </c>
       <c r="L233" t="s">
-        <v>1047</v>
+        <v>43</v>
       </c>
       <c r="M233" t="s">
-        <v>1047</v>
+        <v>43</v>
       </c>
       <c r="N233" t="s">
-        <v>1047</v>
+        <v>43</v>
       </c>
     </row>
     <row r="234">
       <c r="B234" t="s">
-        <v>1883</v>
+        <v>1889</v>
       </c>
       <c r="C234" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="D234" t="s">
         <v>40</v>
@@ -17838,36 +17878,36 @@
         <v>41</v>
       </c>
       <c r="F234" t="s">
-        <v>43</v>
+        <v>1905</v>
       </c>
       <c r="G234" t="s">
-        <v>43</v>
+        <v>1052</v>
       </c>
       <c r="I234" t="s">
-        <v>43</v>
+        <v>1052</v>
       </c>
       <c r="J234" t="s">
-        <v>43</v>
+        <v>1052</v>
       </c>
       <c r="K234" t="s">
-        <v>43</v>
+        <v>1052</v>
       </c>
       <c r="L234" t="s">
-        <v>43</v>
+        <v>1052</v>
       </c>
       <c r="M234" t="s">
-        <v>43</v>
+        <v>1052</v>
       </c>
       <c r="N234" t="s">
-        <v>43</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="235">
       <c r="B235" t="s">
-        <v>1889</v>
+        <v>1891</v>
       </c>
       <c r="C235" t="s">
-        <v>37</v>
+        <v>39</v>
       </c>
       <c r="D235" t="s">
         <v>40</v>
@@ -17876,36 +17916,39 @@
         <v>41</v>
       </c>
       <c r="F235" t="s">
-        <v>1905</v>
+        <v>1900</v>
       </c>
       <c r="G235" t="s">
-        <v>1052</v>
+        <v>1893</v>
+      </c>
+      <c r="H235" t="s">
+        <v>134</v>
       </c>
       <c r="I235" t="s">
-        <v>1052</v>
+        <v>1894</v>
       </c>
       <c r="J235" t="s">
-        <v>1052</v>
+        <v>1895</v>
       </c>
       <c r="K235" t="s">
-        <v>1052</v>
+        <v>1896</v>
       </c>
       <c r="L235" t="s">
-        <v>1052</v>
+        <v>1897</v>
       </c>
       <c r="M235" t="s">
-        <v>1052</v>
+        <v>1898</v>
       </c>
       <c r="N235" t="s">
-        <v>1052</v>
+        <v>1899</v>
       </c>
     </row>
     <row r="236">
       <c r="B236" t="s">
-        <v>1891</v>
+        <v>1901</v>
       </c>
       <c r="C236" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="D236" t="s">
         <v>40</v>
@@ -17914,74 +17957,71 @@
         <v>41</v>
       </c>
       <c r="F236" t="s">
-        <v>1900</v>
+        <v>1902</v>
       </c>
       <c r="G236" t="s">
-        <v>1893</v>
-      </c>
-      <c r="H236" t="s">
-        <v>134</v>
+        <v>1052</v>
       </c>
       <c r="I236" t="s">
-        <v>1894</v>
+        <v>1052</v>
       </c>
       <c r="J236" t="s">
-        <v>1895</v>
+        <v>1052</v>
       </c>
       <c r="K236" t="s">
-        <v>1896</v>
+        <v>1052</v>
       </c>
       <c r="L236" t="s">
-        <v>1897</v>
+        <v>1052</v>
       </c>
       <c r="M236" t="s">
-        <v>1898</v>
+        <v>1052</v>
       </c>
       <c r="N236" t="s">
-        <v>1899</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="237">
       <c r="B237" t="s">
-        <v>1901</v>
+        <v>1908</v>
       </c>
       <c r="C237" t="s">
         <v>37</v>
       </c>
       <c r="D237" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="E237" t="s">
         <v>41</v>
       </c>
       <c r="F237" t="s">
-        <v>1902</v>
+        <v>1909</v>
       </c>
       <c r="G237" t="s">
-        <v>1052</v>
+        <v>43</v>
       </c>
       <c r="I237" t="s">
-        <v>1052</v>
+        <v>43</v>
       </c>
       <c r="J237" t="s">
-        <v>1052</v>
+        <v>43</v>
       </c>
       <c r="K237" t="s">
-        <v>1052</v>
+        <v>43</v>
       </c>
       <c r="L237" t="s">
-        <v>1052</v>
+        <v>43</v>
       </c>
       <c r="M237" t="s">
-        <v>1052</v>
+        <v>43</v>
       </c>
       <c r="N237" t="s">
-        <v>1052</v>
+        <v>43</v>
       </c>
     </row>
     <row r="238">
       <c r="B238" t="s">
-        <v>1908</v>
+        <v>1911</v>
       </c>
       <c r="C238" t="s">
         <v>37</v>
@@ -17993,45 +18033,45 @@
         <v>41</v>
       </c>
       <c r="F238" t="s">
-        <v>1909</v>
+        <v>1915</v>
       </c>
       <c r="G238" t="s">
-        <v>43</v>
+        <v>1052</v>
       </c>
       <c r="I238" t="s">
-        <v>43</v>
+        <v>1052</v>
       </c>
       <c r="J238" t="s">
-        <v>43</v>
+        <v>1052</v>
       </c>
       <c r="K238" t="s">
-        <v>43</v>
+        <v>1052</v>
       </c>
       <c r="L238" t="s">
-        <v>43</v>
+        <v>1052</v>
       </c>
       <c r="M238" t="s">
-        <v>43</v>
+        <v>1052</v>
       </c>
       <c r="N238" t="s">
-        <v>43</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="239">
       <c r="B239" t="s">
-        <v>1911</v>
+        <v>1913</v>
       </c>
       <c r="C239" t="s">
         <v>37</v>
       </c>
       <c r="D239" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="E239" t="s">
         <v>41</v>
       </c>
       <c r="F239" t="s">
-        <v>1915</v>
+        <v>1068</v>
       </c>
       <c r="G239" t="s">
         <v>1052</v>
@@ -18057,19 +18097,19 @@
     </row>
     <row r="240">
       <c r="B240" t="s">
-        <v>1913</v>
+        <v>1916</v>
       </c>
       <c r="C240" t="s">
         <v>37</v>
       </c>
       <c r="D240" t="s">
-        <v>40</v>
+        <v>49</v>
       </c>
       <c r="E240" t="s">
         <v>41</v>
       </c>
       <c r="F240" t="s">
-        <v>1068</v>
+        <v>1918</v>
       </c>
       <c r="G240" t="s">
         <v>1052</v>
@@ -18095,45 +18135,45 @@
     </row>
     <row r="241">
       <c r="B241" t="s">
-        <v>1916</v>
+        <v>1919</v>
       </c>
       <c r="C241" t="s">
         <v>37</v>
       </c>
       <c r="D241" t="s">
-        <v>49</v>
+        <v>40</v>
       </c>
       <c r="E241" t="s">
         <v>41</v>
       </c>
       <c r="F241" t="s">
-        <v>1918</v>
+        <v>1933</v>
       </c>
       <c r="G241" t="s">
-        <v>1052</v>
+        <v>1933</v>
       </c>
       <c r="I241" t="s">
-        <v>1052</v>
+        <v>1933</v>
       </c>
       <c r="J241" t="s">
-        <v>1052</v>
+        <v>1933</v>
       </c>
       <c r="K241" t="s">
-        <v>1052</v>
+        <v>1933</v>
       </c>
       <c r="L241" t="s">
-        <v>1052</v>
+        <v>1933</v>
       </c>
       <c r="M241" t="s">
-        <v>1052</v>
+        <v>1933</v>
       </c>
       <c r="N241" t="s">
-        <v>1052</v>
+        <v>1933</v>
       </c>
     </row>
     <row r="242">
       <c r="B242" t="s">
-        <v>1919</v>
+        <v>1920</v>
       </c>
       <c r="C242" t="s">
         <v>37</v>
@@ -18145,33 +18185,33 @@
         <v>41</v>
       </c>
       <c r="F242" t="s">
-        <v>1933</v>
+        <v>1934</v>
       </c>
       <c r="G242" t="s">
-        <v>1933</v>
+        <v>1934</v>
       </c>
       <c r="I242" t="s">
-        <v>1933</v>
+        <v>1934</v>
       </c>
       <c r="J242" t="s">
-        <v>1933</v>
+        <v>1934</v>
       </c>
       <c r="K242" t="s">
-        <v>1933</v>
+        <v>1934</v>
       </c>
       <c r="L242" t="s">
-        <v>1933</v>
+        <v>1934</v>
       </c>
       <c r="M242" t="s">
-        <v>1933</v>
+        <v>1934</v>
       </c>
       <c r="N242" t="s">
-        <v>1933</v>
+        <v>1934</v>
       </c>
     </row>
     <row r="243">
       <c r="B243" t="s">
-        <v>1920</v>
+        <v>1929</v>
       </c>
       <c r="C243" t="s">
         <v>37</v>
@@ -18183,83 +18223,83 @@
         <v>41</v>
       </c>
       <c r="F243" t="s">
-        <v>1934</v>
+        <v>1935</v>
       </c>
       <c r="G243" t="s">
-        <v>1934</v>
+        <v>1935</v>
       </c>
       <c r="I243" t="s">
-        <v>1934</v>
+        <v>1935</v>
       </c>
       <c r="J243" t="s">
-        <v>1934</v>
+        <v>1935</v>
       </c>
       <c r="K243" t="s">
-        <v>1934</v>
+        <v>1935</v>
       </c>
       <c r="L243" t="s">
-        <v>1934</v>
+        <v>1935</v>
       </c>
       <c r="M243" t="s">
-        <v>1934</v>
+        <v>1935</v>
       </c>
       <c r="N243" t="s">
-        <v>1934</v>
+        <v>1935</v>
       </c>
     </row>
     <row r="244">
       <c r="B244" t="s">
-        <v>1929</v>
+        <v>1936</v>
       </c>
       <c r="C244" t="s">
         <v>37</v>
       </c>
       <c r="D244" t="s">
-        <v>40</v>
+        <v>42</v>
       </c>
       <c r="E244" t="s">
         <v>41</v>
       </c>
       <c r="F244" t="s">
-        <v>1935</v>
+        <v>1052</v>
       </c>
       <c r="G244" t="s">
-        <v>1935</v>
+        <v>1052</v>
       </c>
       <c r="I244" t="s">
-        <v>1935</v>
+        <v>1052</v>
       </c>
       <c r="J244" t="s">
-        <v>1935</v>
+        <v>1052</v>
       </c>
       <c r="K244" t="s">
-        <v>1935</v>
+        <v>1052</v>
       </c>
       <c r="L244" t="s">
-        <v>1935</v>
+        <v>1052</v>
       </c>
       <c r="M244" t="s">
-        <v>1935</v>
+        <v>1052</v>
       </c>
       <c r="N244" t="s">
-        <v>1935</v>
+        <v>1052</v>
       </c>
     </row>
     <row r="245">
       <c r="B245" t="s">
-        <v>1936</v>
+        <v>1938</v>
       </c>
       <c r="C245" t="s">
         <v>37</v>
       </c>
       <c r="D245" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="E245" t="s">
         <v>41</v>
       </c>
       <c r="F245" t="s">
-        <v>1052</v>
+        <v>1939</v>
       </c>
       <c r="G245" t="s">
         <v>1052</v>
@@ -18281,6 +18321,47 @@
       </c>
       <c r="N245" t="s">
         <v>1052</v>
+      </c>
+    </row>
+    <row r="246">
+      <c r="B246" t="s">
+        <v>1940</v>
+      </c>
+      <c r="C246" t="s">
+        <v>38</v>
+      </c>
+      <c r="D246" t="s">
+        <v>40</v>
+      </c>
+      <c r="E246" t="s">
+        <v>41</v>
+      </c>
+      <c r="F246" t="s">
+        <v>1940</v>
+      </c>
+      <c r="G246" t="s">
+        <v>1941</v>
+      </c>
+      <c r="H246" t="s">
+        <v>135</v>
+      </c>
+      <c r="I246" t="s">
+        <v>1942</v>
+      </c>
+      <c r="J246" t="s">
+        <v>1943</v>
+      </c>
+      <c r="K246" t="s">
+        <v>1940</v>
+      </c>
+      <c r="L246" t="s">
+        <v>1944</v>
+      </c>
+      <c r="M246" t="s">
+        <v>1940</v>
+      </c>
+      <c r="N246" t="s">
+        <v>1945</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed Delta issue and timer not updating properly
</commit_message>
<xml_diff>
--- a/RECOVER/assets/texts/texts.xlsx
+++ b/RECOVER/assets/texts/texts.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1389038" uniqueCount="1946">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1404332" uniqueCount="1949">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -6978,6 +6978,15 @@
   </si>
   <si>
     <t xml:space="preserve">настройка</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Delta</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Delta: &lt;&gt;</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Elapsed Time: &lt;value&gt; minutes</t>
   </si>
 </sst>
 </file>
@@ -16725,7 +16734,7 @@
         <v>41</v>
       </c>
       <c r="F205" t="s">
-        <v>1907</v>
+        <v>1948</v>
       </c>
       <c r="G205" t="s">
         <v>1036</v>
@@ -18362,6 +18371,44 @@
       </c>
       <c r="N246" t="s">
         <v>1945</v>
+      </c>
+    </row>
+    <row r="247">
+      <c r="B247" t="s">
+        <v>1946</v>
+      </c>
+      <c r="C247" t="s">
+        <v>76</v>
+      </c>
+      <c r="D247" t="s">
+        <v>42</v>
+      </c>
+      <c r="E247" t="s">
+        <v>41</v>
+      </c>
+      <c r="F247" t="s">
+        <v>1947</v>
+      </c>
+      <c r="G247" t="s">
+        <v>1947</v>
+      </c>
+      <c r="I247" t="s">
+        <v>1947</v>
+      </c>
+      <c r="J247" t="s">
+        <v>1947</v>
+      </c>
+      <c r="K247" t="s">
+        <v>1947</v>
+      </c>
+      <c r="L247" t="s">
+        <v>1947</v>
+      </c>
+      <c r="M247" t="s">
+        <v>1947</v>
+      </c>
+      <c r="N247" t="s">
+        <v>1947</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Fixed issues where binary wasn't correctly figured out.
</commit_message>
<xml_diff>
--- a/RECOVER/assets/texts/texts.xlsx
+++ b/RECOVER/assets/texts/texts.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1404332" uniqueCount="1949">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1409450" uniqueCount="1951">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -6987,6 +6987,12 @@
   </si>
   <si>
     <t xml:space="preserve">Elapsed Time: &lt;value&gt; minutes</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId252</t>
+  </si>
+  <si>
+    <t xml:space="preserve">&lt;&gt;</t>
   </si>
 </sst>
 </file>
@@ -18411,6 +18417,44 @@
         <v>1947</v>
       </c>
     </row>
+    <row r="248">
+      <c r="B248" t="s">
+        <v>1949</v>
+      </c>
+      <c r="C248" t="s">
+        <v>39</v>
+      </c>
+      <c r="D248" t="s">
+        <v>42</v>
+      </c>
+      <c r="E248" t="s">
+        <v>41</v>
+      </c>
+      <c r="F248" t="s">
+        <v>1950</v>
+      </c>
+      <c r="G248" t="s">
+        <v>1950</v>
+      </c>
+      <c r="I248" t="s">
+        <v>1950</v>
+      </c>
+      <c r="J248" t="s">
+        <v>1950</v>
+      </c>
+      <c r="K248" t="s">
+        <v>1950</v>
+      </c>
+      <c r="L248" t="s">
+        <v>1950</v>
+      </c>
+      <c r="M248" t="s">
+        <v>1950</v>
+      </c>
+      <c r="N248" t="s">
+        <v>1950</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>

<commit_message>
Fuming time now calculated on MCU, Fixed issue where full and final precursor was swapped
</commit_message>
<xml_diff>
--- a/RECOVER/assets/texts/texts.xlsx
+++ b/RECOVER/assets/texts/texts.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1456132" uniqueCount="2015">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1497908" uniqueCount="2071">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -7105,6 +7105,230 @@
   </si>
   <si>
     <t xml:space="preserve">无诊断 发现</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aucun diagnostic 
+a trouvé</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sin diagnóstico 
+encontró</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keine diagnose 
+gefunden</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nessuna diagnostica 
+trovato</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sem diagnóstico 
+encontrado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Нет диагностики 
+нашел</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No diagnostics
+found</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aucun diagnostic 
+a trouvé</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sin diagnóstico 
+encontró</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keine diagnose 
+gefunden</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nessuna diagnostica 
+trovato</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sem diagnóstico 
+encontrado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Нет диагностики 
+нашел</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No diagnostics
+found</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aucun diagnostic 
+a trouvé</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sin diagnóstico 
+encontró</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keine diagnose 
+gefunden</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nessuna diagnostica 
+trovato</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sem diagnóstico 
+encontrado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Нет диагностики 
+нашел</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No diagnostics
+found</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aucun diagnostic 
+a trouvé</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sin diagnóstico 
+encontró</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keine diagnose 
+gefunden</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nessuna diagnostica 
+trovato</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sem diagnóstico 
+encontrado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Нет диагностики 
+нашел</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No diagnostics
+found</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aucun diagnostic 
+a trouvé</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sin diagnóstico 
+encontró</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keine diagnose 
+gefunden</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nessuna diagnostica 
+trovato</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sem diagnóstico 
+encontrado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Нет диагностики 
+нашел</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No diagnostics
+found</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aucun diagnostic 
+a trouvé</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sin diagnóstico 
+encontró</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keine diagnose 
+gefunden</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nessuna diagnostica 
+trovato</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sem diagnóstico 
+encontrado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Нет диагностики 
+нашел</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No diagnostics
+found</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aucun diagnostic 
+a trouvé</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sin diagnóstico 
+encontró</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keine diagnose 
+gefunden</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nessuna diagnostica 
+trovato</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sem diagnóstico 
+encontrado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Нет диагностики 
+нашел</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No diagnostics
+found</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aucun diagnostic 
+a trouvé</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sin diagnóstico 
+encontró</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keine diagnose 
+gefunden</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nessuna diagnostica 
+trovato</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sem diagnóstico 
+encontrado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Нет диагностики 
+нашел</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No diagnostics
+found</t>
   </si>
   <si>
     <t xml:space="preserve">Aucun diagnostic 
@@ -18850,7 +19074,7 @@
         <v>41</v>
       </c>
       <c r="F253" t="s">
-        <v>2008</v>
+        <v>2064</v>
       </c>
       <c r="G253" t="s">
         <v>1987</v>
@@ -18859,22 +19083,22 @@
         <v>131</v>
       </c>
       <c r="I253" t="s">
-        <v>2009</v>
+        <v>2065</v>
       </c>
       <c r="J253" t="s">
-        <v>2010</v>
+        <v>2066</v>
       </c>
       <c r="K253" t="s">
-        <v>2011</v>
+        <v>2067</v>
       </c>
       <c r="L253" t="s">
-        <v>2012</v>
+        <v>2068</v>
       </c>
       <c r="M253" t="s">
-        <v>2013</v>
+        <v>2069</v>
       </c>
       <c r="N253" t="s">
-        <v>2014</v>
+        <v>2070</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Allowed user to cancel saving service report via save menu
</commit_message>
<xml_diff>
--- a/RECOVER/assets/texts/texts.xlsx
+++ b/RECOVER/assets/texts/texts.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1518796" uniqueCount="2099">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1529240" uniqueCount="2113">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -7105,6 +7105,62 @@
   </si>
   <si>
     <t xml:space="preserve">无诊断 发现</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aucun diagnostic 
+a trouvé</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sin diagnóstico 
+encontró</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keine diagnose 
+gefunden</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nessuna diagnostica 
+trovato</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sem diagnóstico 
+encontrado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Нет диагностики 
+нашел</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No diagnostics
+found</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Aucun diagnostic 
+a trouvé</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sin diagnóstico 
+encontró</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Keine diagnose 
+gefunden</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Nessuna diagnostica 
+trovato</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Sem diagnóstico 
+encontrado</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Нет диагностики 
+нашел</t>
+  </si>
+  <si>
+    <t xml:space="preserve">No diagnostics
+found</t>
   </si>
   <si>
     <t xml:space="preserve">Aucun diagnostic 
@@ -19186,7 +19242,7 @@
         <v>41</v>
       </c>
       <c r="F253" t="s">
-        <v>2092</v>
+        <v>2106</v>
       </c>
       <c r="G253" t="s">
         <v>1987</v>
@@ -19195,22 +19251,22 @@
         <v>131</v>
       </c>
       <c r="I253" t="s">
-        <v>2093</v>
+        <v>2107</v>
       </c>
       <c r="J253" t="s">
-        <v>2094</v>
+        <v>2108</v>
       </c>
       <c r="K253" t="s">
-        <v>2095</v>
+        <v>2109</v>
       </c>
       <c r="L253" t="s">
-        <v>2096</v>
+        <v>2110</v>
       </c>
       <c r="M253" t="s">
-        <v>2097</v>
+        <v>2111</v>
       </c>
       <c r="N253" t="s">
-        <v>2098</v>
+        <v>2112</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Moved text and fonts to quadspi
</commit_message>
<xml_diff>
--- a/RECOVER/assets/texts/texts.xlsx
+++ b/RECOVER/assets/texts/texts.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1544915" uniqueCount="2150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1550140" uniqueCount="2150">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -15502,25 +15502,25 @@
         <v>331</v>
       </c>
       <c r="G156" t="s">
-        <v>331</v>
+        <v>1047</v>
       </c>
       <c r="I156" t="s">
-        <v>331</v>
+        <v>1047</v>
       </c>
       <c r="J156" t="s">
-        <v>331</v>
+        <v>1047</v>
       </c>
       <c r="K156" t="s">
-        <v>331</v>
+        <v>1047</v>
       </c>
       <c r="L156" t="s">
-        <v>331</v>
+        <v>1047</v>
       </c>
       <c r="M156" t="s">
-        <v>331</v>
+        <v>1047</v>
       </c>
       <c r="N156" t="s">
-        <v>331</v>
+        <v>1047</v>
       </c>
     </row>
     <row r="157" spans="2:14">

</xml_diff>

<commit_message>
Fixed simulator building, Fixed Chinese texts
</commit_message>
<xml_diff>
--- a/RECOVER/assets/texts/texts.xlsx
+++ b/RECOVER/assets/texts/texts.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1550140" uniqueCount="2150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1555367" uniqueCount="2150">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -19013,6 +19013,9 @@
       <c r="G244" t="s">
         <v>1075</v>
       </c>
+      <c r="H244" t="s">
+        <v>131</v>
+      </c>
       <c r="I244" t="s">
         <v>1076</v>
       </c>
@@ -19050,6 +19053,9 @@
       </c>
       <c r="G245" t="s">
         <v>2143</v>
+      </c>
+      <c r="H245" t="s">
+        <v>131</v>
       </c>
       <c r="I245" t="s">
         <v>2144</v>

</xml_diff>

<commit_message>
Add Soak Test 30 runs and make soak test buttons hidden if fume plug is not in
</commit_message>
<xml_diff>
--- a/RECOVER/assets/texts/texts.xlsx
+++ b/RECOVER/assets/texts/texts.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1555367" uniqueCount="2150">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1581662" uniqueCount="2155">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -7716,6 +7716,21 @@
   </si>
   <si>
     <t xml:space="preserve">Начать настройку</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId257</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Start 30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Start Continous</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId258</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fume Override Plug</t>
   </si>
 </sst>
 </file>
@@ -13391,7 +13406,7 @@
         <v>41</v>
       </c>
       <c r="F104" t="s">
-        <v>246</v>
+        <v>2152</v>
       </c>
       <c r="G104" t="s">
         <v>1047</v>
@@ -19393,6 +19408,82 @@
       </c>
       <c r="N253" t="s">
         <v>1993</v>
+      </c>
+    </row>
+    <row r="254">
+      <c r="B254" t="s">
+        <v>2150</v>
+      </c>
+      <c r="C254" t="s">
+        <v>37</v>
+      </c>
+      <c r="D254" t="s">
+        <v>40</v>
+      </c>
+      <c r="E254" t="s">
+        <v>41</v>
+      </c>
+      <c r="F254" t="s">
+        <v>2151</v>
+      </c>
+      <c r="G254" t="s">
+        <v>1047</v>
+      </c>
+      <c r="I254" t="s">
+        <v>1047</v>
+      </c>
+      <c r="J254" t="s">
+        <v>1047</v>
+      </c>
+      <c r="K254" t="s">
+        <v>1047</v>
+      </c>
+      <c r="L254" t="s">
+        <v>1047</v>
+      </c>
+      <c r="M254" t="s">
+        <v>1047</v>
+      </c>
+      <c r="N254" t="s">
+        <v>1047</v>
+      </c>
+    </row>
+    <row r="255">
+      <c r="B255" t="s">
+        <v>2153</v>
+      </c>
+      <c r="C255" t="s">
+        <v>37</v>
+      </c>
+      <c r="D255" t="s">
+        <v>40</v>
+      </c>
+      <c r="E255" t="s">
+        <v>41</v>
+      </c>
+      <c r="F255" t="s">
+        <v>2154</v>
+      </c>
+      <c r="G255" t="s">
+        <v>1047</v>
+      </c>
+      <c r="I255" t="s">
+        <v>1047</v>
+      </c>
+      <c r="J255" t="s">
+        <v>1047</v>
+      </c>
+      <c r="K255" t="s">
+        <v>1047</v>
+      </c>
+      <c r="L255" t="s">
+        <v>1047</v>
+      </c>
+      <c r="M255" t="s">
+        <v>1047</v>
+      </c>
+      <c r="N255" t="s">
+        <v>1047</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Added ability to start drying if process detects moisture
</commit_message>
<xml_diff>
--- a/RECOVER/assets/texts/texts.xlsx
+++ b/RECOVER/assets/texts/texts.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="61557" uniqueCount="1369">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="67454" uniqueCount="1373">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -4359,6 +4359,18 @@
   </si>
   <si>
     <t xml:space="preserve">Română (RO)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId259</t>
+  </si>
+  <si>
+    <t xml:space="preserve">New Text</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId260</t>
+  </si>
+  <si>
+    <t xml:space="preserve">SingleUseId261</t>
   </si>
 </sst>
 </file>
@@ -17063,6 +17075,129 @@
         <v>1368</v>
       </c>
     </row>
+    <row r="257">
+      <c r="B257" t="s">
+        <v>1369</v>
+      </c>
+      <c r="C257" t="s">
+        <v>37</v>
+      </c>
+      <c r="D257" t="s">
+        <v>42</v>
+      </c>
+      <c r="E257" t="s">
+        <v>41</v>
+      </c>
+      <c r="F257" t="s">
+        <v>1370</v>
+      </c>
+      <c r="G257" t="s">
+        <v>1370</v>
+      </c>
+      <c r="I257" t="s">
+        <v>1370</v>
+      </c>
+      <c r="J257" t="s">
+        <v>1370</v>
+      </c>
+      <c r="K257" t="s">
+        <v>1370</v>
+      </c>
+      <c r="L257" t="s">
+        <v>1370</v>
+      </c>
+      <c r="M257" t="s">
+        <v>1370</v>
+      </c>
+      <c r="N257" t="s">
+        <v>1370</v>
+      </c>
+      <c r="V257" t="s">
+        <v>1370</v>
+      </c>
+    </row>
+    <row r="258">
+      <c r="B258" t="s">
+        <v>1371</v>
+      </c>
+      <c r="C258" t="s">
+        <v>37</v>
+      </c>
+      <c r="D258" t="s">
+        <v>42</v>
+      </c>
+      <c r="E258" t="s">
+        <v>41</v>
+      </c>
+      <c r="F258" t="s">
+        <v>1370</v>
+      </c>
+      <c r="G258" t="s">
+        <v>1370</v>
+      </c>
+      <c r="I258" t="s">
+        <v>1370</v>
+      </c>
+      <c r="J258" t="s">
+        <v>1370</v>
+      </c>
+      <c r="K258" t="s">
+        <v>1370</v>
+      </c>
+      <c r="L258" t="s">
+        <v>1370</v>
+      </c>
+      <c r="M258" t="s">
+        <v>1370</v>
+      </c>
+      <c r="N258" t="s">
+        <v>1370</v>
+      </c>
+      <c r="V258" t="s">
+        <v>1370</v>
+      </c>
+    </row>
+    <row r="259">
+      <c r="B259" t="s">
+        <v>1372</v>
+      </c>
+      <c r="C259" t="s">
+        <v>37</v>
+      </c>
+      <c r="D259" t="s">
+        <v>42</v>
+      </c>
+      <c r="E259" t="s">
+        <v>41</v>
+      </c>
+      <c r="F259" t="s">
+        <v>1370</v>
+      </c>
+      <c r="G259" t="s">
+        <v>1370</v>
+      </c>
+      <c r="I259" t="s">
+        <v>1370</v>
+      </c>
+      <c r="J259" t="s">
+        <v>1370</v>
+      </c>
+      <c r="K259" t="s">
+        <v>1370</v>
+      </c>
+      <c r="L259" t="s">
+        <v>1370</v>
+      </c>
+      <c r="M259" t="s">
+        <v>1370</v>
+      </c>
+      <c r="N259" t="s">
+        <v>1370</v>
+      </c>
+      <c r="V259" t="s">
+        <v>1370</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>

<commit_message>
Add Arabic, Polish, Ukranian
</commit_message>
<xml_diff>
--- a/RECOVER/assets/texts/texts.xlsx
+++ b/RECOVER/assets/texts/texts.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102836" uniqueCount="1385">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132838" uniqueCount="1397">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -4419,6 +4419,42 @@
   <si>
     <t xml:space="preserve">Attempting to clear the excess moisture.
 Please wait...</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Language_AR</t>
+  </si>
+  <si>
+    <t xml:space="preserve">عربي (AR)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Language_PL</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Polski (PL)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Language_UA</t>
+  </si>
+  <si>
+    <t xml:space="preserve">українська (UA)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">AR-TYPOGRAPHY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">PL-TYPOGRAPHY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UA-TYPOGRAPHY</t>
   </si>
 </sst>
 </file>
@@ -6293,6 +6329,24 @@
       <c r="W3" t="s">
         <v>1365</v>
       </c>
+      <c r="X3" t="s">
+        <v>1385</v>
+      </c>
+      <c r="Y3" t="s">
+        <v>1386</v>
+      </c>
+      <c r="Z3" t="s">
+        <v>1387</v>
+      </c>
+      <c r="AA3" t="s">
+        <v>1394</v>
+      </c>
+      <c r="AB3" t="s">
+        <v>1395</v>
+      </c>
+      <c r="AC3" t="s">
+        <v>1396</v>
+      </c>
     </row>
     <row r="4" spans="2:22">
       <c r="B4" t="s">
@@ -6346,6 +6400,15 @@
       <c r="V4" t="s">
         <v>1258</v>
       </c>
+      <c r="X4" t="s">
+        <v>55</v>
+      </c>
+      <c r="Y4" t="s">
+        <v>55</v>
+      </c>
+      <c r="Z4" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="5" spans="2:22">
       <c r="B5" t="s">
@@ -6396,6 +6459,15 @@
       <c r="V5" t="s">
         <v>1259</v>
       </c>
+      <c r="X5" t="s">
+        <v>381</v>
+      </c>
+      <c r="Y5" t="s">
+        <v>381</v>
+      </c>
+      <c r="Z5" t="s">
+        <v>381</v>
+      </c>
     </row>
     <row r="6" spans="2:22">
       <c r="B6" t="s">
@@ -6443,6 +6515,15 @@
       <c r="V6" t="s">
         <v>1260</v>
       </c>
+      <c r="X6" t="s">
+        <v>382</v>
+      </c>
+      <c r="Y6" t="s">
+        <v>382</v>
+      </c>
+      <c r="Z6" t="s">
+        <v>382</v>
+      </c>
     </row>
     <row r="7" spans="2:22">
       <c r="B7" t="s">
@@ -6487,6 +6568,15 @@
       <c r="V7" t="s">
         <v>1261</v>
       </c>
+      <c r="X7" t="s">
+        <v>59</v>
+      </c>
+      <c r="Y7" t="s">
+        <v>59</v>
+      </c>
+      <c r="Z7" t="s">
+        <v>59</v>
+      </c>
     </row>
     <row r="8" spans="2:22" ht="26.25">
       <c r="B8" t="s">
@@ -6531,6 +6621,15 @@
       <c r="V8" t="s">
         <v>1262</v>
       </c>
+      <c r="X8" t="s">
+        <v>383</v>
+      </c>
+      <c r="Y8" t="s">
+        <v>383</v>
+      </c>
+      <c r="Z8" t="s">
+        <v>383</v>
+      </c>
     </row>
     <row r="9" spans="2:22">
       <c r="B9" t="s">
@@ -6581,6 +6680,15 @@
       <c r="V9" t="s">
         <v>1263</v>
       </c>
+      <c r="X9" t="s">
+        <v>61</v>
+      </c>
+      <c r="Y9" t="s">
+        <v>61</v>
+      </c>
+      <c r="Z9" t="s">
+        <v>61</v>
+      </c>
     </row>
     <row r="10" spans="2:22">
       <c r="B10" t="s">
@@ -6643,6 +6751,15 @@
       <c r="V10" t="s">
         <v>1264</v>
       </c>
+      <c r="X10" t="s">
+        <v>62</v>
+      </c>
+      <c r="Y10" t="s">
+        <v>62</v>
+      </c>
+      <c r="Z10" t="s">
+        <v>62</v>
+      </c>
     </row>
     <row r="11" spans="2:22">
       <c r="B11" t="s">
@@ -6687,6 +6804,15 @@
       <c r="V11" t="s">
         <v>1265</v>
       </c>
+      <c r="X11" t="s">
+        <v>80</v>
+      </c>
+      <c r="Y11" t="s">
+        <v>80</v>
+      </c>
+      <c r="Z11" t="s">
+        <v>80</v>
+      </c>
     </row>
     <row r="12" spans="2:22">
       <c r="B12" t="s">
@@ -6731,6 +6857,15 @@
       <c r="V12" t="s">
         <v>1266</v>
       </c>
+      <c r="X12" t="s">
+        <v>66</v>
+      </c>
+      <c r="Y12" t="s">
+        <v>66</v>
+      </c>
+      <c r="Z12" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="13" spans="2:22">
       <c r="B13" t="s">
@@ -6775,6 +6910,15 @@
       <c r="V13" t="s">
         <v>1267</v>
       </c>
+      <c r="X13" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y13" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z13" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="14" spans="2:22">
       <c r="B14" t="s">
@@ -6816,6 +6960,15 @@
       <c r="V14" t="s">
         <v>70</v>
       </c>
+      <c r="X14" t="s">
+        <v>70</v>
+      </c>
+      <c r="Y14" t="s">
+        <v>70</v>
+      </c>
+      <c r="Z14" t="s">
+        <v>70</v>
+      </c>
     </row>
     <row r="15" spans="2:22">
       <c r="B15" t="s">
@@ -6857,6 +7010,15 @@
       <c r="V15" t="s">
         <v>72</v>
       </c>
+      <c r="X15" t="s">
+        <v>72</v>
+      </c>
+      <c r="Y15" t="s">
+        <v>72</v>
+      </c>
+      <c r="Z15" t="s">
+        <v>72</v>
+      </c>
     </row>
     <row r="16" spans="2:22">
       <c r="B16" t="s">
@@ -6898,6 +7060,15 @@
       <c r="V16" t="s">
         <v>75</v>
       </c>
+      <c r="X16" t="s">
+        <v>75</v>
+      </c>
+      <c r="Y16" t="s">
+        <v>75</v>
+      </c>
+      <c r="Z16" t="s">
+        <v>75</v>
+      </c>
     </row>
     <row r="17" spans="2:22">
       <c r="B17" t="s">
@@ -6939,6 +7110,15 @@
       <c r="V17" t="s">
         <v>43</v>
       </c>
+      <c r="X17" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y17" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z17" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="18" spans="2:22">
       <c r="B18" t="s">
@@ -6980,6 +7160,15 @@
       <c r="V18" t="s">
         <v>43</v>
       </c>
+      <c r="X18" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y18" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z18" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="19" spans="2:22">
       <c r="B19" t="s">
@@ -7021,6 +7210,15 @@
       <c r="V19" t="s">
         <v>1025</v>
       </c>
+      <c r="X19" t="s">
+        <v>82</v>
+      </c>
+      <c r="Y19" t="s">
+        <v>82</v>
+      </c>
+      <c r="Z19" t="s">
+        <v>82</v>
+      </c>
     </row>
     <row r="20" spans="2:22">
       <c r="B20" t="s">
@@ -7062,6 +7260,15 @@
       <c r="V20" t="s">
         <v>85</v>
       </c>
+      <c r="X20" t="s">
+        <v>85</v>
+      </c>
+      <c r="Y20" t="s">
+        <v>85</v>
+      </c>
+      <c r="Z20" t="s">
+        <v>85</v>
+      </c>
     </row>
     <row r="21" spans="2:22">
       <c r="B21" t="s">
@@ -7103,6 +7310,15 @@
       <c r="V21" t="s">
         <v>1025</v>
       </c>
+      <c r="X21" t="s">
+        <v>87</v>
+      </c>
+      <c r="Y21" t="s">
+        <v>87</v>
+      </c>
+      <c r="Z21" t="s">
+        <v>87</v>
+      </c>
     </row>
     <row r="22" spans="2:22">
       <c r="B22" t="s">
@@ -7144,6 +7360,15 @@
       <c r="V22" t="s">
         <v>1025</v>
       </c>
+      <c r="X22" t="s">
+        <v>48</v>
+      </c>
+      <c r="Y22" t="s">
+        <v>48</v>
+      </c>
+      <c r="Z22" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="23" spans="2:22">
       <c r="B23" t="s">
@@ -7185,6 +7410,15 @@
       <c r="V23" t="s">
         <v>128</v>
       </c>
+      <c r="X23" t="s">
+        <v>128</v>
+      </c>
+      <c r="Y23" t="s">
+        <v>128</v>
+      </c>
+      <c r="Z23" t="s">
+        <v>128</v>
+      </c>
     </row>
     <row r="24" spans="2:22">
       <c r="B24" t="s">
@@ -7229,6 +7463,15 @@
       <c r="V24" t="s">
         <v>1268</v>
       </c>
+      <c r="X24" t="s">
+        <v>118</v>
+      </c>
+      <c r="Y24" t="s">
+        <v>118</v>
+      </c>
+      <c r="Z24" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="25" spans="2:22">
       <c r="B25" t="s">
@@ -7270,6 +7513,15 @@
       <c r="V25" t="s">
         <v>472</v>
       </c>
+      <c r="X25" t="s">
+        <v>472</v>
+      </c>
+      <c r="Y25" t="s">
+        <v>472</v>
+      </c>
+      <c r="Z25" t="s">
+        <v>472</v>
+      </c>
     </row>
     <row r="26" spans="2:22">
       <c r="B26" t="s">
@@ -7338,6 +7590,24 @@
       <c r="W26" t="s">
         <v>129</v>
       </c>
+      <c r="X26" t="s">
+        <v>939</v>
+      </c>
+      <c r="Y26" t="s">
+        <v>939</v>
+      </c>
+      <c r="Z26" t="s">
+        <v>939</v>
+      </c>
+      <c r="AA26" t="s">
+        <v>129</v>
+      </c>
+      <c r="AB26" t="s">
+        <v>129</v>
+      </c>
+      <c r="AC26" t="s">
+        <v>129</v>
+      </c>
     </row>
     <row r="27" spans="2:22">
       <c r="B27" t="s">
@@ -7379,6 +7649,15 @@
       <c r="V27" t="s">
         <v>473</v>
       </c>
+      <c r="X27" t="s">
+        <v>473</v>
+      </c>
+      <c r="Y27" t="s">
+        <v>473</v>
+      </c>
+      <c r="Z27" t="s">
+        <v>473</v>
+      </c>
     </row>
     <row r="28" spans="2:22">
       <c r="B28" t="s">
@@ -7420,6 +7699,15 @@
       <c r="V28" t="s">
         <v>474</v>
       </c>
+      <c r="X28" t="s">
+        <v>474</v>
+      </c>
+      <c r="Y28" t="s">
+        <v>474</v>
+      </c>
+      <c r="Z28" t="s">
+        <v>474</v>
+      </c>
     </row>
     <row r="29" spans="2:22">
       <c r="B29" t="s">
@@ -7461,6 +7749,15 @@
       <c r="V29" t="s">
         <v>475</v>
       </c>
+      <c r="X29" t="s">
+        <v>475</v>
+      </c>
+      <c r="Y29" t="s">
+        <v>475</v>
+      </c>
+      <c r="Z29" t="s">
+        <v>475</v>
+      </c>
     </row>
     <row r="30" spans="2:22">
       <c r="B30" t="s">
@@ -7502,6 +7799,15 @@
       <c r="V30" t="s">
         <v>476</v>
       </c>
+      <c r="X30" t="s">
+        <v>476</v>
+      </c>
+      <c r="Y30" t="s">
+        <v>476</v>
+      </c>
+      <c r="Z30" t="s">
+        <v>476</v>
+      </c>
     </row>
     <row r="31" spans="2:22">
       <c r="B31" t="s">
@@ -7543,6 +7849,15 @@
       <c r="V31" t="s">
         <v>1025</v>
       </c>
+      <c r="X31" t="s">
+        <v>101</v>
+      </c>
+      <c r="Y31" t="s">
+        <v>101</v>
+      </c>
+      <c r="Z31" t="s">
+        <v>101</v>
+      </c>
     </row>
     <row r="32" spans="2:22">
       <c r="B32" t="s">
@@ -7584,6 +7899,15 @@
       <c r="V32" t="s">
         <v>1025</v>
       </c>
+      <c r="X32" t="s">
+        <v>103</v>
+      </c>
+      <c r="Y32" t="s">
+        <v>103</v>
+      </c>
+      <c r="Z32" t="s">
+        <v>103</v>
+      </c>
     </row>
     <row r="33" spans="2:22">
       <c r="B33" t="s">
@@ -7625,6 +7949,15 @@
       <c r="V33" t="s">
         <v>1025</v>
       </c>
+      <c r="X33" t="s">
+        <v>363</v>
+      </c>
+      <c r="Y33" t="s">
+        <v>363</v>
+      </c>
+      <c r="Z33" t="s">
+        <v>363</v>
+      </c>
     </row>
     <row r="34" spans="2:22">
       <c r="B34" t="s">
@@ -7666,6 +7999,15 @@
       <c r="V34" t="s">
         <v>1025</v>
       </c>
+      <c r="X34" t="s">
+        <v>105</v>
+      </c>
+      <c r="Y34" t="s">
+        <v>105</v>
+      </c>
+      <c r="Z34" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="35" spans="2:22">
       <c r="B35" t="s">
@@ -7707,6 +8049,15 @@
       <c r="V35" t="s">
         <v>1025</v>
       </c>
+      <c r="X35" t="s">
+        <v>164</v>
+      </c>
+      <c r="Y35" t="s">
+        <v>164</v>
+      </c>
+      <c r="Z35" t="s">
+        <v>164</v>
+      </c>
     </row>
     <row r="36" spans="2:22">
       <c r="B36" t="s">
@@ -7748,6 +8099,15 @@
       <c r="V36" t="s">
         <v>1025</v>
       </c>
+      <c r="X36" t="s">
+        <v>166</v>
+      </c>
+      <c r="Y36" t="s">
+        <v>166</v>
+      </c>
+      <c r="Z36" t="s">
+        <v>166</v>
+      </c>
     </row>
     <row r="37" spans="2:22">
       <c r="B37" t="s">
@@ -7789,6 +8149,15 @@
       <c r="V37" t="s">
         <v>1025</v>
       </c>
+      <c r="X37" t="s">
+        <v>165</v>
+      </c>
+      <c r="Y37" t="s">
+        <v>165</v>
+      </c>
+      <c r="Z37" t="s">
+        <v>165</v>
+      </c>
     </row>
     <row r="38" spans="2:22">
       <c r="B38" t="s">
@@ -7830,6 +8199,15 @@
       <c r="V38" t="s">
         <v>1025</v>
       </c>
+      <c r="X38" t="s">
+        <v>110</v>
+      </c>
+      <c r="Y38" t="s">
+        <v>110</v>
+      </c>
+      <c r="Z38" t="s">
+        <v>110</v>
+      </c>
     </row>
     <row r="39" spans="2:22">
       <c r="B39" t="s">
@@ -7871,6 +8249,15 @@
       <c r="V39" t="s">
         <v>1025</v>
       </c>
+      <c r="X39" t="s">
+        <v>112</v>
+      </c>
+      <c r="Y39" t="s">
+        <v>112</v>
+      </c>
+      <c r="Z39" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="40" spans="2:22">
       <c r="B40" t="s">
@@ -7912,6 +8299,15 @@
       <c r="V40" t="s">
         <v>1025</v>
       </c>
+      <c r="X40" t="s">
+        <v>117</v>
+      </c>
+      <c r="Y40" t="s">
+        <v>117</v>
+      </c>
+      <c r="Z40" t="s">
+        <v>117</v>
+      </c>
     </row>
     <row r="41" spans="2:22">
       <c r="B41" t="s">
@@ -7953,6 +8349,15 @@
       <c r="V41" t="s">
         <v>1025</v>
       </c>
+      <c r="X41" t="s">
+        <v>115</v>
+      </c>
+      <c r="Y41" t="s">
+        <v>115</v>
+      </c>
+      <c r="Z41" t="s">
+        <v>115</v>
+      </c>
     </row>
     <row r="42" spans="2:22">
       <c r="B42" t="s">
@@ -7994,6 +8399,15 @@
       <c r="V42" t="s">
         <v>1025</v>
       </c>
+      <c r="X42" t="s">
+        <v>362</v>
+      </c>
+      <c r="Y42" t="s">
+        <v>362</v>
+      </c>
+      <c r="Z42" t="s">
+        <v>362</v>
+      </c>
     </row>
     <row r="43" spans="2:22">
       <c r="B43" t="s">
@@ -8038,6 +8452,15 @@
       <c r="V43" t="s">
         <v>1269</v>
       </c>
+      <c r="X43" t="s">
+        <v>52</v>
+      </c>
+      <c r="Y43" t="s">
+        <v>52</v>
+      </c>
+      <c r="Z43" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="44" spans="2:22">
       <c r="B44" t="s">
@@ -8082,6 +8505,15 @@
       <c r="V44" t="s">
         <v>1270</v>
       </c>
+      <c r="X44" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y44" t="s">
+        <v>53</v>
+      </c>
+      <c r="Z44" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="45" spans="2:22">
       <c r="B45" t="s">
@@ -8129,6 +8561,15 @@
       <c r="V45" t="s">
         <v>1271</v>
       </c>
+      <c r="X45" t="s">
+        <v>134</v>
+      </c>
+      <c r="Y45" t="s">
+        <v>134</v>
+      </c>
+      <c r="Z45" t="s">
+        <v>134</v>
+      </c>
     </row>
     <row r="46" spans="2:22">
       <c r="B46" t="s">
@@ -8173,6 +8614,15 @@
       <c r="V46" t="s">
         <v>136</v>
       </c>
+      <c r="X46" t="s">
+        <v>136</v>
+      </c>
+      <c r="Y46" t="s">
+        <v>136</v>
+      </c>
+      <c r="Z46" t="s">
+        <v>136</v>
+      </c>
     </row>
     <row r="47" spans="2:22">
       <c r="B47" t="s">
@@ -8214,6 +8664,15 @@
       <c r="V47" t="s">
         <v>1025</v>
       </c>
+      <c r="X47" t="s">
+        <v>139</v>
+      </c>
+      <c r="Y47" t="s">
+        <v>139</v>
+      </c>
+      <c r="Z47" t="s">
+        <v>139</v>
+      </c>
     </row>
     <row r="48" spans="2:22">
       <c r="B48" t="s">
@@ -8255,6 +8714,15 @@
       <c r="V48" t="s">
         <v>1026</v>
       </c>
+      <c r="X48" t="s">
+        <v>118</v>
+      </c>
+      <c r="Y48" t="s">
+        <v>118</v>
+      </c>
+      <c r="Z48" t="s">
+        <v>118</v>
+      </c>
     </row>
     <row r="49" spans="2:22">
       <c r="B49" t="s">
@@ -8296,6 +8764,15 @@
       <c r="V49" t="s">
         <v>1027</v>
       </c>
+      <c r="X49" t="s">
+        <v>124</v>
+      </c>
+      <c r="Y49" t="s">
+        <v>124</v>
+      </c>
+      <c r="Z49" t="s">
+        <v>124</v>
+      </c>
     </row>
     <row r="50" spans="2:22">
       <c r="B50" t="s">
@@ -8337,6 +8814,15 @@
       <c r="V50" t="s">
         <v>1027</v>
       </c>
+      <c r="X50" t="s">
+        <v>126</v>
+      </c>
+      <c r="Y50" t="s">
+        <v>126</v>
+      </c>
+      <c r="Z50" t="s">
+        <v>126</v>
+      </c>
     </row>
     <row r="51" spans="2:22">
       <c r="B51" t="s">
@@ -8378,6 +8864,15 @@
       <c r="V51" t="s">
         <v>1026</v>
       </c>
+      <c r="X51" t="s">
+        <v>119</v>
+      </c>
+      <c r="Y51" t="s">
+        <v>119</v>
+      </c>
+      <c r="Z51" t="s">
+        <v>119</v>
+      </c>
     </row>
     <row r="52" spans="2:22">
       <c r="B52" t="s">
@@ -8419,6 +8914,15 @@
       <c r="V52" t="s">
         <v>1027</v>
       </c>
+      <c r="X52" t="s">
+        <v>149</v>
+      </c>
+      <c r="Y52" t="s">
+        <v>149</v>
+      </c>
+      <c r="Z52" t="s">
+        <v>149</v>
+      </c>
     </row>
     <row r="53" spans="2:22">
       <c r="B53" t="s">
@@ -8460,6 +8964,15 @@
       <c r="V53" t="s">
         <v>1026</v>
       </c>
+      <c r="X53" t="s">
+        <v>245</v>
+      </c>
+      <c r="Y53" t="s">
+        <v>245</v>
+      </c>
+      <c r="Z53" t="s">
+        <v>245</v>
+      </c>
     </row>
     <row r="54" spans="2:22">
       <c r="B54" t="s">
@@ -8501,6 +9014,15 @@
       <c r="V54" t="s">
         <v>1026</v>
       </c>
+      <c r="X54" t="s">
+        <v>120</v>
+      </c>
+      <c r="Y54" t="s">
+        <v>120</v>
+      </c>
+      <c r="Z54" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="55" spans="2:22">
       <c r="B55" t="s">
@@ -8542,6 +9064,15 @@
       <c r="V55" t="s">
         <v>1026</v>
       </c>
+      <c r="X55" t="s">
+        <v>121</v>
+      </c>
+      <c r="Y55" t="s">
+        <v>121</v>
+      </c>
+      <c r="Z55" t="s">
+        <v>121</v>
+      </c>
     </row>
     <row r="56" spans="2:22">
       <c r="B56" t="s">
@@ -8583,6 +9114,15 @@
       <c r="V56" t="s">
         <v>1026</v>
       </c>
+      <c r="X56" t="s">
+        <v>122</v>
+      </c>
+      <c r="Y56" t="s">
+        <v>122</v>
+      </c>
+      <c r="Z56" t="s">
+        <v>122</v>
+      </c>
     </row>
     <row r="57" spans="2:22">
       <c r="B57" t="s">
@@ -8624,6 +9164,15 @@
       <c r="V57" t="s">
         <v>1026</v>
       </c>
+      <c r="X57" t="s">
+        <v>123</v>
+      </c>
+      <c r="Y57" t="s">
+        <v>123</v>
+      </c>
+      <c r="Z57" t="s">
+        <v>123</v>
+      </c>
     </row>
     <row r="58" spans="2:22">
       <c r="B58" t="s">
@@ -8665,6 +9214,15 @@
       <c r="V58" t="s">
         <v>1026</v>
       </c>
+      <c r="X58" t="s">
+        <v>137</v>
+      </c>
+      <c r="Y58" t="s">
+        <v>137</v>
+      </c>
+      <c r="Z58" t="s">
+        <v>137</v>
+      </c>
     </row>
     <row r="59" spans="2:22">
       <c r="B59" t="s">
@@ -8709,6 +9267,15 @@
       <c r="V59" t="s">
         <v>1272</v>
       </c>
+      <c r="X59" t="s">
+        <v>90</v>
+      </c>
+      <c r="Y59" t="s">
+        <v>90</v>
+      </c>
+      <c r="Z59" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="60" spans="2:22">
       <c r="B60" t="s">
@@ -8750,6 +9317,15 @@
       <c r="V60" t="s">
         <v>1273</v>
       </c>
+      <c r="X60" t="s">
+        <v>153</v>
+      </c>
+      <c r="Y60" t="s">
+        <v>153</v>
+      </c>
+      <c r="Z60" t="s">
+        <v>153</v>
+      </c>
     </row>
     <row r="61" spans="2:22">
       <c r="B61" t="s">
@@ -8791,6 +9367,15 @@
       <c r="V61" t="s">
         <v>1025</v>
       </c>
+      <c r="X61" t="s">
+        <v>154</v>
+      </c>
+      <c r="Y61" t="s">
+        <v>154</v>
+      </c>
+      <c r="Z61" t="s">
+        <v>154</v>
+      </c>
     </row>
     <row r="62" spans="2:22">
       <c r="B62" t="s">
@@ -8832,6 +9417,15 @@
       <c r="V62" t="s">
         <v>1025</v>
       </c>
+      <c r="X62" t="s">
+        <v>156</v>
+      </c>
+      <c r="Y62" t="s">
+        <v>156</v>
+      </c>
+      <c r="Z62" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="63" spans="2:22">
       <c r="B63" t="s">
@@ -8873,6 +9467,15 @@
       <c r="V63" t="s">
         <v>1274</v>
       </c>
+      <c r="X63" t="s">
+        <v>158</v>
+      </c>
+      <c r="Y63" t="s">
+        <v>158</v>
+      </c>
+      <c r="Z63" t="s">
+        <v>158</v>
+      </c>
     </row>
     <row r="64" spans="2:22">
       <c r="B64" t="s">
@@ -8914,6 +9517,15 @@
       <c r="V64" t="s">
         <v>1025</v>
       </c>
+      <c r="X64" t="s">
+        <v>163</v>
+      </c>
+      <c r="Y64" t="s">
+        <v>163</v>
+      </c>
+      <c r="Z64" t="s">
+        <v>163</v>
+      </c>
     </row>
     <row r="65" spans="2:22" ht="26.25">
       <c r="B65" t="s">
@@ -8958,6 +9570,15 @@
       <c r="V65" t="s">
         <v>1275</v>
       </c>
+      <c r="X65" t="s">
+        <v>384</v>
+      </c>
+      <c r="Y65" t="s">
+        <v>384</v>
+      </c>
+      <c r="Z65" t="s">
+        <v>384</v>
+      </c>
     </row>
     <row r="66" spans="2:22" ht="26.25">
       <c r="B66" t="s">
@@ -9002,6 +9623,15 @@
       <c r="V66" t="s">
         <v>1276</v>
       </c>
+      <c r="X66" t="s">
+        <v>385</v>
+      </c>
+      <c r="Y66" t="s">
+        <v>385</v>
+      </c>
+      <c r="Z66" t="s">
+        <v>385</v>
+      </c>
     </row>
     <row r="67" spans="2:22" ht="26.25">
       <c r="B67" t="s">
@@ -9046,6 +9676,15 @@
       <c r="V67" t="s">
         <v>1277</v>
       </c>
+      <c r="X67" t="s">
+        <v>386</v>
+      </c>
+      <c r="Y67" t="s">
+        <v>386</v>
+      </c>
+      <c r="Z67" t="s">
+        <v>386</v>
+      </c>
     </row>
     <row r="68" spans="2:22">
       <c r="B68" t="s">
@@ -9090,6 +9729,15 @@
       <c r="V68" t="s">
         <v>1278</v>
       </c>
+      <c r="X68" t="s">
+        <v>387</v>
+      </c>
+      <c r="Y68" t="s">
+        <v>387</v>
+      </c>
+      <c r="Z68" t="s">
+        <v>387</v>
+      </c>
     </row>
     <row r="69" spans="2:22">
       <c r="B69" t="s">
@@ -9134,6 +9782,15 @@
       <c r="V69" t="s">
         <v>1279</v>
       </c>
+      <c r="X69" t="s">
+        <v>388</v>
+      </c>
+      <c r="Y69" t="s">
+        <v>388</v>
+      </c>
+      <c r="Z69" t="s">
+        <v>388</v>
+      </c>
     </row>
     <row r="70" spans="2:22">
       <c r="B70" t="s">
@@ -9175,6 +9832,15 @@
       <c r="V70" t="s">
         <v>43</v>
       </c>
+      <c r="X70" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y70" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z70" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="71" spans="2:22">
       <c r="B71" t="s">
@@ -9219,6 +9885,15 @@
       <c r="V71" t="s">
         <v>1280</v>
       </c>
+      <c r="X71" t="s">
+        <v>389</v>
+      </c>
+      <c r="Y71" t="s">
+        <v>389</v>
+      </c>
+      <c r="Z71" t="s">
+        <v>389</v>
+      </c>
     </row>
     <row r="72" spans="2:22">
       <c r="B72" t="s">
@@ -9260,6 +9935,15 @@
       <c r="V72" t="s">
         <v>1025</v>
       </c>
+      <c r="X72" t="s">
+        <v>178</v>
+      </c>
+      <c r="Y72" t="s">
+        <v>178</v>
+      </c>
+      <c r="Z72" t="s">
+        <v>178</v>
+      </c>
     </row>
     <row r="73" spans="2:22">
       <c r="B73" t="s">
@@ -9301,6 +9985,15 @@
       <c r="V73" t="s">
         <v>1025</v>
       </c>
+      <c r="X73" t="s">
+        <v>177</v>
+      </c>
+      <c r="Y73" t="s">
+        <v>177</v>
+      </c>
+      <c r="Z73" t="s">
+        <v>177</v>
+      </c>
     </row>
     <row r="74" spans="2:22">
       <c r="B74" t="s">
@@ -9342,6 +10035,15 @@
       <c r="V74" t="s">
         <v>43</v>
       </c>
+      <c r="X74" t="s">
+        <v>191</v>
+      </c>
+      <c r="Y74" t="s">
+        <v>191</v>
+      </c>
+      <c r="Z74" t="s">
+        <v>191</v>
+      </c>
     </row>
     <row r="75" spans="2:22">
       <c r="B75" t="s">
@@ -9383,6 +10085,15 @@
       <c r="V75" t="s">
         <v>43</v>
       </c>
+      <c r="X75" t="s">
+        <v>192</v>
+      </c>
+      <c r="Y75" t="s">
+        <v>192</v>
+      </c>
+      <c r="Z75" t="s">
+        <v>192</v>
+      </c>
     </row>
     <row r="76" spans="2:22">
       <c r="B76" t="s">
@@ -9424,6 +10135,15 @@
       <c r="V76" t="s">
         <v>43</v>
       </c>
+      <c r="X76" t="s">
+        <v>193</v>
+      </c>
+      <c r="Y76" t="s">
+        <v>193</v>
+      </c>
+      <c r="Z76" t="s">
+        <v>193</v>
+      </c>
     </row>
     <row r="77" spans="2:22">
       <c r="B77" t="s">
@@ -9465,6 +10185,15 @@
       <c r="V77" t="s">
         <v>43</v>
       </c>
+      <c r="X77" t="s">
+        <v>194</v>
+      </c>
+      <c r="Y77" t="s">
+        <v>194</v>
+      </c>
+      <c r="Z77" t="s">
+        <v>194</v>
+      </c>
     </row>
     <row r="78" spans="2:22">
       <c r="B78" t="s">
@@ -9506,6 +10235,15 @@
       <c r="V78" t="s">
         <v>43</v>
       </c>
+      <c r="X78" t="s">
+        <v>195</v>
+      </c>
+      <c r="Y78" t="s">
+        <v>195</v>
+      </c>
+      <c r="Z78" t="s">
+        <v>195</v>
+      </c>
     </row>
     <row r="79" spans="2:22">
       <c r="B79" t="s">
@@ -9547,6 +10285,15 @@
       <c r="V79" t="s">
         <v>43</v>
       </c>
+      <c r="X79" t="s">
+        <v>196</v>
+      </c>
+      <c r="Y79" t="s">
+        <v>196</v>
+      </c>
+      <c r="Z79" t="s">
+        <v>196</v>
+      </c>
     </row>
     <row r="80" spans="2:22">
       <c r="B80" t="s">
@@ -9588,6 +10335,15 @@
       <c r="V80" t="s">
         <v>43</v>
       </c>
+      <c r="X80" t="s">
+        <v>197</v>
+      </c>
+      <c r="Y80" t="s">
+        <v>197</v>
+      </c>
+      <c r="Z80" t="s">
+        <v>197</v>
+      </c>
     </row>
     <row r="81" spans="2:22">
       <c r="B81" t="s">
@@ -9629,6 +10385,15 @@
       <c r="V81" t="s">
         <v>43</v>
       </c>
+      <c r="X81" t="s">
+        <v>198</v>
+      </c>
+      <c r="Y81" t="s">
+        <v>198</v>
+      </c>
+      <c r="Z81" t="s">
+        <v>198</v>
+      </c>
     </row>
     <row r="82" spans="2:22">
       <c r="B82" t="s">
@@ -9670,6 +10435,15 @@
       <c r="V82" t="s">
         <v>43</v>
       </c>
+      <c r="X82" t="s">
+        <v>199</v>
+      </c>
+      <c r="Y82" t="s">
+        <v>199</v>
+      </c>
+      <c r="Z82" t="s">
+        <v>199</v>
+      </c>
     </row>
     <row r="83" spans="2:22">
       <c r="B83" t="s">
@@ -9711,6 +10485,15 @@
       <c r="V83" t="s">
         <v>43</v>
       </c>
+      <c r="X83" t="s">
+        <v>200</v>
+      </c>
+      <c r="Y83" t="s">
+        <v>200</v>
+      </c>
+      <c r="Z83" t="s">
+        <v>200</v>
+      </c>
     </row>
     <row r="84" spans="2:22">
       <c r="B84" t="s">
@@ -9752,6 +10535,15 @@
       <c r="V84" t="s">
         <v>43</v>
       </c>
+      <c r="X84" t="s">
+        <v>201</v>
+      </c>
+      <c r="Y84" t="s">
+        <v>201</v>
+      </c>
+      <c r="Z84" t="s">
+        <v>201</v>
+      </c>
     </row>
     <row r="85" spans="2:22">
       <c r="B85" t="s">
@@ -9793,6 +10585,15 @@
       <c r="V85" t="s">
         <v>43</v>
       </c>
+      <c r="X85" t="s">
+        <v>202</v>
+      </c>
+      <c r="Y85" t="s">
+        <v>202</v>
+      </c>
+      <c r="Z85" t="s">
+        <v>202</v>
+      </c>
     </row>
     <row r="86" spans="2:22">
       <c r="B86" t="s">
@@ -9834,6 +10635,15 @@
       <c r="V86" t="s">
         <v>1025</v>
       </c>
+      <c r="X86" t="s">
+        <v>205</v>
+      </c>
+      <c r="Y86" t="s">
+        <v>205</v>
+      </c>
+      <c r="Z86" t="s">
+        <v>205</v>
+      </c>
     </row>
     <row r="87" spans="2:22">
       <c r="B87" t="s">
@@ -9875,6 +10685,15 @@
       <c r="V87" t="s">
         <v>1025</v>
       </c>
+      <c r="X87" t="s">
+        <v>156</v>
+      </c>
+      <c r="Y87" t="s">
+        <v>156</v>
+      </c>
+      <c r="Z87" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="88" spans="2:22">
       <c r="B88" t="s">
@@ -9916,6 +10735,15 @@
       <c r="V88" t="s">
         <v>1025</v>
       </c>
+      <c r="X88" t="s">
+        <v>209</v>
+      </c>
+      <c r="Y88" t="s">
+        <v>209</v>
+      </c>
+      <c r="Z88" t="s">
+        <v>209</v>
+      </c>
     </row>
     <row r="89" spans="2:22">
       <c r="B89" t="s">
@@ -9957,6 +10785,15 @@
       <c r="V89" t="s">
         <v>1025</v>
       </c>
+      <c r="X89" t="s">
+        <v>211</v>
+      </c>
+      <c r="Y89" t="s">
+        <v>211</v>
+      </c>
+      <c r="Z89" t="s">
+        <v>211</v>
+      </c>
     </row>
     <row r="90" spans="2:22">
       <c r="B90" t="s">
@@ -9998,6 +10835,15 @@
       <c r="V90" t="s">
         <v>1025</v>
       </c>
+      <c r="X90" t="s">
+        <v>247</v>
+      </c>
+      <c r="Y90" t="s">
+        <v>247</v>
+      </c>
+      <c r="Z90" t="s">
+        <v>247</v>
+      </c>
     </row>
     <row r="91" spans="2:22">
       <c r="B91" t="s">
@@ -10039,6 +10885,15 @@
       <c r="V91" t="s">
         <v>1025</v>
       </c>
+      <c r="X91" t="s">
+        <v>143</v>
+      </c>
+      <c r="Y91" t="s">
+        <v>143</v>
+      </c>
+      <c r="Z91" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="92" spans="2:22">
       <c r="B92" t="s">
@@ -10080,6 +10935,15 @@
       <c r="V92" t="s">
         <v>1025</v>
       </c>
+      <c r="X92" t="s">
+        <v>219</v>
+      </c>
+      <c r="Y92" t="s">
+        <v>219</v>
+      </c>
+      <c r="Z92" t="s">
+        <v>219</v>
+      </c>
     </row>
     <row r="93" spans="2:22">
       <c r="B93" t="s">
@@ -10121,6 +10985,15 @@
       <c r="V93" t="s">
         <v>1025</v>
       </c>
+      <c r="X93" t="s">
+        <v>220</v>
+      </c>
+      <c r="Y93" t="s">
+        <v>220</v>
+      </c>
+      <c r="Z93" t="s">
+        <v>220</v>
+      </c>
     </row>
     <row r="94" spans="2:22">
       <c r="B94" t="s">
@@ -10162,6 +11035,15 @@
       <c r="V94" t="s">
         <v>1025</v>
       </c>
+      <c r="X94" t="s">
+        <v>221</v>
+      </c>
+      <c r="Y94" t="s">
+        <v>221</v>
+      </c>
+      <c r="Z94" t="s">
+        <v>221</v>
+      </c>
     </row>
     <row r="95" spans="2:22">
       <c r="B95" t="s">
@@ -10203,6 +11085,15 @@
       <c r="V95" t="s">
         <v>1025</v>
       </c>
+      <c r="X95" t="s">
+        <v>222</v>
+      </c>
+      <c r="Y95" t="s">
+        <v>222</v>
+      </c>
+      <c r="Z95" t="s">
+        <v>222</v>
+      </c>
     </row>
     <row r="96" spans="2:22">
       <c r="B96" t="s">
@@ -10244,6 +11135,15 @@
       <c r="V96" t="s">
         <v>1025</v>
       </c>
+      <c r="X96" t="s">
+        <v>224</v>
+      </c>
+      <c r="Y96" t="s">
+        <v>224</v>
+      </c>
+      <c r="Z96" t="s">
+        <v>224</v>
+      </c>
     </row>
     <row r="97" spans="2:22">
       <c r="B97" t="s">
@@ -10285,6 +11185,15 @@
       <c r="V97" t="s">
         <v>1025</v>
       </c>
+      <c r="X97" t="s">
+        <v>225</v>
+      </c>
+      <c r="Y97" t="s">
+        <v>225</v>
+      </c>
+      <c r="Z97" t="s">
+        <v>225</v>
+      </c>
     </row>
     <row r="98" spans="2:22">
       <c r="B98" t="s">
@@ -10326,6 +11235,15 @@
       <c r="V98" t="s">
         <v>1025</v>
       </c>
+      <c r="X98" t="s">
+        <v>227</v>
+      </c>
+      <c r="Y98" t="s">
+        <v>227</v>
+      </c>
+      <c r="Z98" t="s">
+        <v>227</v>
+      </c>
     </row>
     <row r="99" spans="2:22" ht="26.25">
       <c r="B99" t="s">
@@ -10367,6 +11285,15 @@
       <c r="V99" t="s">
         <v>1281</v>
       </c>
+      <c r="X99" t="s">
+        <v>229</v>
+      </c>
+      <c r="Y99" t="s">
+        <v>229</v>
+      </c>
+      <c r="Z99" t="s">
+        <v>229</v>
+      </c>
     </row>
     <row r="100" spans="2:22">
       <c r="B100" t="s">
@@ -10408,6 +11335,15 @@
       <c r="V100" t="s">
         <v>1282</v>
       </c>
+      <c r="X100" t="s">
+        <v>249</v>
+      </c>
+      <c r="Y100" t="s">
+        <v>249</v>
+      </c>
+      <c r="Z100" t="s">
+        <v>249</v>
+      </c>
     </row>
     <row r="101" spans="2:22" ht="26.25">
       <c r="B101" t="s">
@@ -10449,6 +11385,15 @@
       <c r="V101" t="s">
         <v>1283</v>
       </c>
+      <c r="X101" t="s">
+        <v>250</v>
+      </c>
+      <c r="Y101" t="s">
+        <v>250</v>
+      </c>
+      <c r="Z101" t="s">
+        <v>250</v>
+      </c>
     </row>
     <row r="102" spans="2:22">
       <c r="B102" t="s">
@@ -10490,6 +11435,15 @@
       <c r="V102" t="s">
         <v>1025</v>
       </c>
+      <c r="X102" t="s">
+        <v>233</v>
+      </c>
+      <c r="Y102" t="s">
+        <v>233</v>
+      </c>
+      <c r="Z102" t="s">
+        <v>233</v>
+      </c>
     </row>
     <row r="103" spans="2:22">
       <c r="B103" t="s">
@@ -10531,6 +11485,15 @@
       <c r="V103" t="s">
         <v>43</v>
       </c>
+      <c r="X103" t="s">
+        <v>235</v>
+      </c>
+      <c r="Y103" t="s">
+        <v>235</v>
+      </c>
+      <c r="Z103" t="s">
+        <v>235</v>
+      </c>
     </row>
     <row r="104" spans="2:22">
       <c r="B104" t="s">
@@ -10572,6 +11535,15 @@
       <c r="V104" t="s">
         <v>1025</v>
       </c>
+      <c r="X104" t="s">
+        <v>1254</v>
+      </c>
+      <c r="Y104" t="s">
+        <v>1254</v>
+      </c>
+      <c r="Z104" t="s">
+        <v>1254</v>
+      </c>
     </row>
     <row r="105" spans="2:22">
       <c r="B105" t="s">
@@ -10613,6 +11585,15 @@
       <c r="V105" t="s">
         <v>1025</v>
       </c>
+      <c r="X105" t="s">
+        <v>156</v>
+      </c>
+      <c r="Y105" t="s">
+        <v>156</v>
+      </c>
+      <c r="Z105" t="s">
+        <v>156</v>
+      </c>
     </row>
     <row r="106" spans="2:22">
       <c r="B106" t="s">
@@ -10654,6 +11635,15 @@
       <c r="V106" t="s">
         <v>43</v>
       </c>
+      <c r="X106" t="s">
+        <v>120</v>
+      </c>
+      <c r="Y106" t="s">
+        <v>120</v>
+      </c>
+      <c r="Z106" t="s">
+        <v>120</v>
+      </c>
     </row>
     <row r="107" spans="2:22">
       <c r="B107" t="s">
@@ -10695,6 +11685,15 @@
       <c r="V107" t="s">
         <v>1025</v>
       </c>
+      <c r="X107" t="s">
+        <v>241</v>
+      </c>
+      <c r="Y107" t="s">
+        <v>241</v>
+      </c>
+      <c r="Z107" t="s">
+        <v>241</v>
+      </c>
     </row>
     <row r="108" spans="2:22">
       <c r="B108" t="s">
@@ -10736,6 +11735,15 @@
       <c r="V108" t="s">
         <v>43</v>
       </c>
+      <c r="X108" t="s">
+        <v>246</v>
+      </c>
+      <c r="Y108" t="s">
+        <v>246</v>
+      </c>
+      <c r="Z108" t="s">
+        <v>246</v>
+      </c>
     </row>
     <row r="109" spans="2:22">
       <c r="B109" t="s">
@@ -10777,6 +11785,15 @@
       <c r="V109" t="s">
         <v>43</v>
       </c>
+      <c r="X109" t="s">
+        <v>248</v>
+      </c>
+      <c r="Y109" t="s">
+        <v>248</v>
+      </c>
+      <c r="Z109" t="s">
+        <v>248</v>
+      </c>
     </row>
     <row r="110" spans="2:22">
       <c r="B110" t="s">
@@ -10821,6 +11838,15 @@
       <c r="V110" t="s">
         <v>1284</v>
       </c>
+      <c r="X110" t="s">
+        <v>252</v>
+      </c>
+      <c r="Y110" t="s">
+        <v>252</v>
+      </c>
+      <c r="Z110" t="s">
+        <v>252</v>
+      </c>
     </row>
     <row r="111" spans="2:22">
       <c r="B111" t="s">
@@ -10865,6 +11891,15 @@
       <c r="V111" t="s">
         <v>1285</v>
       </c>
+      <c r="X111" t="s">
+        <v>254</v>
+      </c>
+      <c r="Y111" t="s">
+        <v>254</v>
+      </c>
+      <c r="Z111" t="s">
+        <v>254</v>
+      </c>
     </row>
     <row r="112" spans="2:22">
       <c r="B112" t="s">
@@ -10909,6 +11944,15 @@
       <c r="V112" t="s">
         <v>43</v>
       </c>
+      <c r="X112" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y112" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z112" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="113" spans="2:22">
       <c r="B113" t="s">
@@ -10953,6 +11997,15 @@
       <c r="V113" t="s">
         <v>1286</v>
       </c>
+      <c r="X113" t="s">
+        <v>278</v>
+      </c>
+      <c r="Y113" t="s">
+        <v>278</v>
+      </c>
+      <c r="Z113" t="s">
+        <v>278</v>
+      </c>
     </row>
     <row r="114" spans="2:22">
       <c r="B114" t="s">
@@ -10997,6 +12050,15 @@
       <c r="V114" t="s">
         <v>1287</v>
       </c>
+      <c r="X114" t="s">
+        <v>277</v>
+      </c>
+      <c r="Y114" t="s">
+        <v>277</v>
+      </c>
+      <c r="Z114" t="s">
+        <v>277</v>
+      </c>
     </row>
     <row r="115" spans="2:22">
       <c r="B115" t="s">
@@ -11041,6 +12103,15 @@
       <c r="V115" t="s">
         <v>1288</v>
       </c>
+      <c r="X115" t="s">
+        <v>257</v>
+      </c>
+      <c r="Y115" t="s">
+        <v>257</v>
+      </c>
+      <c r="Z115" t="s">
+        <v>257</v>
+      </c>
     </row>
     <row r="116" spans="2:22">
       <c r="B116" t="s">
@@ -11085,6 +12156,15 @@
       <c r="V116" t="s">
         <v>1289</v>
       </c>
+      <c r="X116" t="s">
+        <v>255</v>
+      </c>
+      <c r="Y116" t="s">
+        <v>255</v>
+      </c>
+      <c r="Z116" t="s">
+        <v>255</v>
+      </c>
     </row>
     <row r="117" spans="2:22">
       <c r="B117" t="s">
@@ -11129,6 +12209,15 @@
       <c r="V117" t="s">
         <v>1290</v>
       </c>
+      <c r="X117" t="s">
+        <v>256</v>
+      </c>
+      <c r="Y117" t="s">
+        <v>256</v>
+      </c>
+      <c r="Z117" t="s">
+        <v>256</v>
+      </c>
     </row>
     <row r="118" spans="2:22">
       <c r="B118" t="s">
@@ -11173,6 +12262,15 @@
       <c r="V118" t="s">
         <v>1291</v>
       </c>
+      <c r="X118" t="s">
+        <v>279</v>
+      </c>
+      <c r="Y118" t="s">
+        <v>279</v>
+      </c>
+      <c r="Z118" t="s">
+        <v>279</v>
+      </c>
     </row>
     <row r="119" spans="2:22">
       <c r="B119" t="s">
@@ -11217,6 +12315,15 @@
       <c r="V119" t="s">
         <v>1292</v>
       </c>
+      <c r="X119" t="s">
+        <v>276</v>
+      </c>
+      <c r="Y119" t="s">
+        <v>276</v>
+      </c>
+      <c r="Z119" t="s">
+        <v>276</v>
+      </c>
     </row>
     <row r="120" spans="2:22">
       <c r="B120" t="s">
@@ -11258,6 +12365,15 @@
       <c r="V120" t="s">
         <v>43</v>
       </c>
+      <c r="X120" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y120" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z120" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="121" spans="2:22">
       <c r="B121" t="s">
@@ -11299,6 +12415,15 @@
       <c r="V121" t="s">
         <v>43</v>
       </c>
+      <c r="X121" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y121" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z121" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="122" spans="2:22">
       <c r="B122" t="s">
@@ -11343,6 +12468,15 @@
       <c r="V122" t="s">
         <v>1293</v>
       </c>
+      <c r="X122" t="s">
+        <v>261</v>
+      </c>
+      <c r="Y122" t="s">
+        <v>261</v>
+      </c>
+      <c r="Z122" t="s">
+        <v>261</v>
+      </c>
     </row>
     <row r="123" spans="2:22">
       <c r="B123" t="s">
@@ -11387,6 +12521,15 @@
       <c r="V123" t="s">
         <v>1294</v>
       </c>
+      <c r="X123" t="s">
+        <v>263</v>
+      </c>
+      <c r="Y123" t="s">
+        <v>263</v>
+      </c>
+      <c r="Z123" t="s">
+        <v>263</v>
+      </c>
     </row>
     <row r="124" spans="2:22">
       <c r="B124" t="s">
@@ -11431,6 +12574,15 @@
       <c r="V124" t="s">
         <v>1269</v>
       </c>
+      <c r="X124" t="s">
+        <v>52</v>
+      </c>
+      <c r="Y124" t="s">
+        <v>52</v>
+      </c>
+      <c r="Z124" t="s">
+        <v>52</v>
+      </c>
     </row>
     <row r="125" spans="2:22">
       <c r="B125" t="s">
@@ -11475,6 +12627,15 @@
       <c r="V125" t="s">
         <v>1270</v>
       </c>
+      <c r="X125" t="s">
+        <v>53</v>
+      </c>
+      <c r="Y125" t="s">
+        <v>53</v>
+      </c>
+      <c r="Z125" t="s">
+        <v>53</v>
+      </c>
     </row>
     <row r="126" spans="2:22">
       <c r="B126" t="s">
@@ -11519,6 +12680,15 @@
       <c r="V126" t="s">
         <v>1295</v>
       </c>
+      <c r="X126" t="s">
+        <v>390</v>
+      </c>
+      <c r="Y126" t="s">
+        <v>390</v>
+      </c>
+      <c r="Z126" t="s">
+        <v>390</v>
+      </c>
     </row>
     <row r="127" spans="2:22">
       <c r="B127" t="s">
@@ -11563,6 +12733,15 @@
       <c r="V127" t="s">
         <v>1296</v>
       </c>
+      <c r="X127" t="s">
+        <v>268</v>
+      </c>
+      <c r="Y127" t="s">
+        <v>268</v>
+      </c>
+      <c r="Z127" t="s">
+        <v>268</v>
+      </c>
     </row>
     <row r="128" spans="2:22">
       <c r="B128" t="s">
@@ -11604,6 +12783,15 @@
       <c r="V128" t="s">
         <v>1025</v>
       </c>
+      <c r="X128" t="s">
+        <v>143</v>
+      </c>
+      <c r="Y128" t="s">
+        <v>143</v>
+      </c>
+      <c r="Z128" t="s">
+        <v>143</v>
+      </c>
     </row>
     <row r="129" spans="2:22">
       <c r="B129" t="s">
@@ -11645,6 +12833,15 @@
       <c r="V129" t="s">
         <v>1025</v>
       </c>
+      <c r="X129" t="s">
+        <v>273</v>
+      </c>
+      <c r="Y129" t="s">
+        <v>273</v>
+      </c>
+      <c r="Z129" t="s">
+        <v>273</v>
+      </c>
     </row>
     <row r="130" spans="2:22">
       <c r="B130" t="s">
@@ -11686,6 +12883,15 @@
       <c r="V130" t="s">
         <v>1025</v>
       </c>
+      <c r="X130" t="s">
+        <v>272</v>
+      </c>
+      <c r="Y130" t="s">
+        <v>272</v>
+      </c>
+      <c r="Z130" t="s">
+        <v>272</v>
+      </c>
     </row>
     <row r="131" spans="2:22">
       <c r="B131" t="s">
@@ -11727,6 +12933,15 @@
       <c r="V131" t="s">
         <v>43</v>
       </c>
+      <c r="X131" t="s">
+        <v>275</v>
+      </c>
+      <c r="Y131" t="s">
+        <v>275</v>
+      </c>
+      <c r="Z131" t="s">
+        <v>275</v>
+      </c>
     </row>
     <row r="132" spans="2:22" ht="26.25">
       <c r="B132" t="s">
@@ -11789,6 +13004,15 @@
       <c r="V132" t="s">
         <v>1297</v>
       </c>
+      <c r="X132" t="s">
+        <v>281</v>
+      </c>
+      <c r="Y132" t="s">
+        <v>281</v>
+      </c>
+      <c r="Z132" t="s">
+        <v>281</v>
+      </c>
     </row>
     <row r="133" spans="2:22">
       <c r="B133" t="s">
@@ -11833,6 +13057,15 @@
       <c r="V133" t="s">
         <v>1298</v>
       </c>
+      <c r="X133" t="s">
+        <v>287</v>
+      </c>
+      <c r="Y133" t="s">
+        <v>287</v>
+      </c>
+      <c r="Z133" t="s">
+        <v>287</v>
+      </c>
     </row>
     <row r="134" spans="2:22">
       <c r="B134" t="s">
@@ -11874,6 +13107,15 @@
       <c r="V134" t="s">
         <v>43</v>
       </c>
+      <c r="X134" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y134" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z134" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="135" spans="2:22" ht="26.25">
       <c r="B135" t="s">
@@ -11918,6 +13160,15 @@
       <c r="V135" t="s">
         <v>1299</v>
       </c>
+      <c r="X135" t="s">
+        <v>391</v>
+      </c>
+      <c r="Y135" t="s">
+        <v>391</v>
+      </c>
+      <c r="Z135" t="s">
+        <v>391</v>
+      </c>
     </row>
     <row r="136" spans="2:22" ht="26.25">
       <c r="B136" t="s">
@@ -11962,6 +13213,15 @@
       <c r="V136" t="s">
         <v>1300</v>
       </c>
+      <c r="X136" t="s">
+        <v>286</v>
+      </c>
+      <c r="Y136" t="s">
+        <v>286</v>
+      </c>
+      <c r="Z136" t="s">
+        <v>286</v>
+      </c>
     </row>
     <row r="137" spans="2:22">
       <c r="B137" t="s">
@@ -12003,6 +13263,15 @@
       <c r="V137" t="s">
         <v>43</v>
       </c>
+      <c r="X137" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y137" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z137" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="138" spans="2:22">
       <c r="B138" t="s">
@@ -12047,6 +13316,15 @@
       <c r="V138" t="s">
         <v>1301</v>
       </c>
+      <c r="X138" t="s">
+        <v>300</v>
+      </c>
+      <c r="Y138" t="s">
+        <v>300</v>
+      </c>
+      <c r="Z138" t="s">
+        <v>300</v>
+      </c>
     </row>
     <row r="139" spans="2:22">
       <c r="B139" t="s">
@@ -12091,6 +13369,15 @@
       <c r="V139" t="s">
         <v>1302</v>
       </c>
+      <c r="X139" t="s">
+        <v>301</v>
+      </c>
+      <c r="Y139" t="s">
+        <v>301</v>
+      </c>
+      <c r="Z139" t="s">
+        <v>301</v>
+      </c>
     </row>
     <row r="140" spans="2:22">
       <c r="B140" t="s">
@@ -12135,6 +13422,15 @@
       <c r="V140" t="s">
         <v>1303</v>
       </c>
+      <c r="X140" t="s">
+        <v>302</v>
+      </c>
+      <c r="Y140" t="s">
+        <v>302</v>
+      </c>
+      <c r="Z140" t="s">
+        <v>302</v>
+      </c>
     </row>
     <row r="141" spans="2:22">
       <c r="B141" t="s">
@@ -12179,6 +13475,15 @@
       <c r="V141" t="s">
         <v>1304</v>
       </c>
+      <c r="X141" t="s">
+        <v>303</v>
+      </c>
+      <c r="Y141" t="s">
+        <v>303</v>
+      </c>
+      <c r="Z141" t="s">
+        <v>303</v>
+      </c>
     </row>
     <row r="142" spans="2:22">
       <c r="B142" t="s">
@@ -12223,6 +13528,15 @@
       <c r="V142" t="s">
         <v>622</v>
       </c>
+      <c r="X142" t="s">
+        <v>304</v>
+      </c>
+      <c r="Y142" t="s">
+        <v>304</v>
+      </c>
+      <c r="Z142" t="s">
+        <v>304</v>
+      </c>
     </row>
     <row r="143" spans="2:22">
       <c r="B143" t="s">
@@ -12267,6 +13581,15 @@
       <c r="V143" t="s">
         <v>1305</v>
       </c>
+      <c r="X143" t="s">
+        <v>305</v>
+      </c>
+      <c r="Y143" t="s">
+        <v>305</v>
+      </c>
+      <c r="Z143" t="s">
+        <v>305</v>
+      </c>
     </row>
     <row r="144" spans="2:22">
       <c r="B144" t="s">
@@ -12311,6 +13634,15 @@
       <c r="V144" t="s">
         <v>1306</v>
       </c>
+      <c r="X144" t="s">
+        <v>306</v>
+      </c>
+      <c r="Y144" t="s">
+        <v>306</v>
+      </c>
+      <c r="Z144" t="s">
+        <v>306</v>
+      </c>
     </row>
     <row r="145" spans="2:22">
       <c r="B145" t="s">
@@ -12355,6 +13687,15 @@
       <c r="V145" t="s">
         <v>1307</v>
       </c>
+      <c r="X145" t="s">
+        <v>307</v>
+      </c>
+      <c r="Y145" t="s">
+        <v>307</v>
+      </c>
+      <c r="Z145" t="s">
+        <v>307</v>
+      </c>
     </row>
     <row r="146" spans="2:22">
       <c r="B146" t="s">
@@ -12399,6 +13740,15 @@
       <c r="V146" t="s">
         <v>1308</v>
       </c>
+      <c r="X146" t="s">
+        <v>308</v>
+      </c>
+      <c r="Y146" t="s">
+        <v>308</v>
+      </c>
+      <c r="Z146" t="s">
+        <v>308</v>
+      </c>
     </row>
     <row r="147" spans="2:22">
       <c r="B147" t="s">
@@ -12443,6 +13793,15 @@
       <c r="V147" t="s">
         <v>1309</v>
       </c>
+      <c r="X147" t="s">
+        <v>309</v>
+      </c>
+      <c r="Y147" t="s">
+        <v>309</v>
+      </c>
+      <c r="Z147" t="s">
+        <v>309</v>
+      </c>
     </row>
     <row r="148" spans="2:22">
       <c r="B148" t="s">
@@ -12487,6 +13846,15 @@
       <c r="V148" t="s">
         <v>1310</v>
       </c>
+      <c r="X148" t="s">
+        <v>310</v>
+      </c>
+      <c r="Y148" t="s">
+        <v>310</v>
+      </c>
+      <c r="Z148" t="s">
+        <v>310</v>
+      </c>
     </row>
     <row r="149" spans="2:22">
       <c r="B149" t="s">
@@ -12531,6 +13899,15 @@
       <c r="V149" t="s">
         <v>1311</v>
       </c>
+      <c r="X149" t="s">
+        <v>311</v>
+      </c>
+      <c r="Y149" t="s">
+        <v>311</v>
+      </c>
+      <c r="Z149" t="s">
+        <v>311</v>
+      </c>
     </row>
     <row r="150" spans="2:22">
       <c r="B150" t="s">
@@ -12575,6 +13952,15 @@
       <c r="V150" t="s">
         <v>1312</v>
       </c>
+      <c r="X150" t="s">
+        <v>314</v>
+      </c>
+      <c r="Y150" t="s">
+        <v>314</v>
+      </c>
+      <c r="Z150" t="s">
+        <v>314</v>
+      </c>
     </row>
     <row r="151" spans="2:22">
       <c r="B151" t="s">
@@ -12619,6 +14005,15 @@
       <c r="V151" t="s">
         <v>1313</v>
       </c>
+      <c r="X151" t="s">
+        <v>315</v>
+      </c>
+      <c r="Y151" t="s">
+        <v>315</v>
+      </c>
+      <c r="Z151" t="s">
+        <v>315</v>
+      </c>
     </row>
     <row r="152" spans="2:22" ht="26.25">
       <c r="B152" t="s">
@@ -12663,6 +14058,15 @@
       <c r="V152" t="s">
         <v>1314</v>
       </c>
+      <c r="X152" t="s">
+        <v>317</v>
+      </c>
+      <c r="Y152" t="s">
+        <v>317</v>
+      </c>
+      <c r="Z152" t="s">
+        <v>317</v>
+      </c>
     </row>
     <row r="153" spans="2:22" ht="26.25">
       <c r="B153" t="s">
@@ -12707,6 +14111,15 @@
       <c r="V153" t="s">
         <v>1315</v>
       </c>
+      <c r="X153" t="s">
+        <v>319</v>
+      </c>
+      <c r="Y153" t="s">
+        <v>319</v>
+      </c>
+      <c r="Z153" t="s">
+        <v>319</v>
+      </c>
     </row>
     <row r="154" spans="2:22">
       <c r="B154" t="s">
@@ -12751,6 +14164,15 @@
       <c r="V154" t="s">
         <v>1316</v>
       </c>
+      <c r="X154" t="s">
+        <v>160</v>
+      </c>
+      <c r="Y154" t="s">
+        <v>160</v>
+      </c>
+      <c r="Z154" t="s">
+        <v>160</v>
+      </c>
     </row>
     <row r="155" spans="2:22">
       <c r="B155" t="s">
@@ -12795,6 +14217,15 @@
       <c r="V155" t="s">
         <v>1317</v>
       </c>
+      <c r="X155" t="s">
+        <v>159</v>
+      </c>
+      <c r="Y155" t="s">
+        <v>159</v>
+      </c>
+      <c r="Z155" t="s">
+        <v>159</v>
+      </c>
     </row>
     <row r="156" spans="2:22">
       <c r="B156" t="s">
@@ -12836,6 +14267,15 @@
       <c r="V156" t="s">
         <v>1025</v>
       </c>
+      <c r="X156" t="s">
+        <v>323</v>
+      </c>
+      <c r="Y156" t="s">
+        <v>323</v>
+      </c>
+      <c r="Z156" t="s">
+        <v>323</v>
+      </c>
     </row>
     <row r="157" spans="2:22">
       <c r="B157" t="s">
@@ -12880,6 +14320,15 @@
       <c r="V157" t="s">
         <v>1318</v>
       </c>
+      <c r="X157" t="s">
+        <v>325</v>
+      </c>
+      <c r="Y157" t="s">
+        <v>325</v>
+      </c>
+      <c r="Z157" t="s">
+        <v>325</v>
+      </c>
     </row>
     <row r="158" spans="2:22">
       <c r="B158" t="s">
@@ -12924,6 +14373,15 @@
       <c r="V158" t="s">
         <v>326</v>
       </c>
+      <c r="X158" t="s">
+        <v>326</v>
+      </c>
+      <c r="Y158" t="s">
+        <v>326</v>
+      </c>
+      <c r="Z158" t="s">
+        <v>326</v>
+      </c>
     </row>
     <row r="159" spans="2:22">
       <c r="B159" t="s">
@@ -12968,6 +14426,15 @@
       <c r="V159" t="s">
         <v>1319</v>
       </c>
+      <c r="X159" t="s">
+        <v>327</v>
+      </c>
+      <c r="Y159" t="s">
+        <v>327</v>
+      </c>
+      <c r="Z159" t="s">
+        <v>327</v>
+      </c>
     </row>
     <row r="160" spans="2:22">
       <c r="B160" t="s">
@@ -13009,6 +14476,15 @@
       <c r="V160" t="s">
         <v>43</v>
       </c>
+      <c r="X160" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y160" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z160" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="161" spans="2:22">
       <c r="B161" t="s">
@@ -13050,6 +14526,15 @@
       <c r="V161" t="s">
         <v>43</v>
       </c>
+      <c r="X161" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y161" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z161" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="162" spans="2:22">
       <c r="B162" t="s">
@@ -13094,6 +14579,15 @@
       <c r="V162" t="s">
         <v>1316</v>
       </c>
+      <c r="X162" t="s">
+        <v>331</v>
+      </c>
+      <c r="Y162" t="s">
+        <v>331</v>
+      </c>
+      <c r="Z162" t="s">
+        <v>331</v>
+      </c>
     </row>
     <row r="163" spans="2:22">
       <c r="B163" t="s">
@@ -13138,6 +14632,15 @@
       <c r="V163" t="s">
         <v>1320</v>
       </c>
+      <c r="X163" t="s">
+        <v>330</v>
+      </c>
+      <c r="Y163" t="s">
+        <v>330</v>
+      </c>
+      <c r="Z163" t="s">
+        <v>330</v>
+      </c>
     </row>
     <row r="164" spans="2:22">
       <c r="B164" t="s">
@@ -13182,6 +14685,15 @@
       <c r="V164" t="s">
         <v>1321</v>
       </c>
+      <c r="X164" t="s">
+        <v>335</v>
+      </c>
+      <c r="Y164" t="s">
+        <v>335</v>
+      </c>
+      <c r="Z164" t="s">
+        <v>335</v>
+      </c>
     </row>
     <row r="165" spans="2:22">
       <c r="B165" t="s">
@@ -13226,6 +14738,15 @@
       <c r="V165" t="s">
         <v>1322</v>
       </c>
+      <c r="X165" t="s">
+        <v>337</v>
+      </c>
+      <c r="Y165" t="s">
+        <v>337</v>
+      </c>
+      <c r="Z165" t="s">
+        <v>337</v>
+      </c>
     </row>
     <row r="166" spans="2:22">
       <c r="B166" t="s">
@@ -13267,6 +14788,15 @@
       <c r="V166" t="s">
         <v>392</v>
       </c>
+      <c r="X166" t="s">
+        <v>392</v>
+      </c>
+      <c r="Y166" t="s">
+        <v>392</v>
+      </c>
+      <c r="Z166" t="s">
+        <v>392</v>
+      </c>
     </row>
     <row r="167" spans="2:22">
       <c r="B167" t="s">
@@ -13308,6 +14838,15 @@
       <c r="V167" t="s">
         <v>393</v>
       </c>
+      <c r="X167" t="s">
+        <v>393</v>
+      </c>
+      <c r="Y167" t="s">
+        <v>393</v>
+      </c>
+      <c r="Z167" t="s">
+        <v>393</v>
+      </c>
     </row>
     <row r="168" spans="2:22">
       <c r="B168" t="s">
@@ -13349,6 +14888,15 @@
       <c r="V168" t="s">
         <v>394</v>
       </c>
+      <c r="X168" t="s">
+        <v>394</v>
+      </c>
+      <c r="Y168" t="s">
+        <v>394</v>
+      </c>
+      <c r="Z168" t="s">
+        <v>394</v>
+      </c>
     </row>
     <row r="169" spans="2:22">
       <c r="B169" t="s">
@@ -13393,6 +14941,15 @@
       <c r="V169" t="s">
         <v>1323</v>
       </c>
+      <c r="X169" t="s">
+        <v>339</v>
+      </c>
+      <c r="Y169" t="s">
+        <v>339</v>
+      </c>
+      <c r="Z169" t="s">
+        <v>339</v>
+      </c>
     </row>
     <row r="170" spans="2:22">
       <c r="B170" t="s">
@@ -13437,6 +14994,15 @@
       <c r="V170" t="s">
         <v>1324</v>
       </c>
+      <c r="X170" t="s">
+        <v>341</v>
+      </c>
+      <c r="Y170" t="s">
+        <v>341</v>
+      </c>
+      <c r="Z170" t="s">
+        <v>341</v>
+      </c>
     </row>
     <row r="171" spans="2:22">
       <c r="B171" t="s">
@@ -13478,6 +15044,15 @@
       <c r="V171" t="s">
         <v>395</v>
       </c>
+      <c r="X171" t="s">
+        <v>395</v>
+      </c>
+      <c r="Y171" t="s">
+        <v>395</v>
+      </c>
+      <c r="Z171" t="s">
+        <v>395</v>
+      </c>
     </row>
     <row r="172" spans="2:22" ht="26.25">
       <c r="B172" t="s">
@@ -13522,6 +15097,15 @@
       <c r="V172" t="s">
         <v>1325</v>
       </c>
+      <c r="X172" t="s">
+        <v>396</v>
+      </c>
+      <c r="Y172" t="s">
+        <v>396</v>
+      </c>
+      <c r="Z172" t="s">
+        <v>396</v>
+      </c>
     </row>
     <row r="173" spans="2:22" ht="26.25">
       <c r="B173" t="s">
@@ -13566,6 +15150,15 @@
       <c r="V173" t="s">
         <v>1326</v>
       </c>
+      <c r="X173" t="s">
+        <v>348</v>
+      </c>
+      <c r="Y173" t="s">
+        <v>348</v>
+      </c>
+      <c r="Z173" t="s">
+        <v>348</v>
+      </c>
     </row>
     <row r="174" spans="2:22">
       <c r="B174" t="s">
@@ -13610,6 +15203,15 @@
       <c r="V174" t="s">
         <v>1327</v>
       </c>
+      <c r="X174" t="s">
+        <v>349</v>
+      </c>
+      <c r="Y174" t="s">
+        <v>349</v>
+      </c>
+      <c r="Z174" t="s">
+        <v>349</v>
+      </c>
     </row>
     <row r="175" spans="2:22" ht="26.25">
       <c r="B175" t="s">
@@ -13654,6 +15256,15 @@
       <c r="V175" t="s">
         <v>1326</v>
       </c>
+      <c r="X175" t="s">
+        <v>352</v>
+      </c>
+      <c r="Y175" t="s">
+        <v>352</v>
+      </c>
+      <c r="Z175" t="s">
+        <v>352</v>
+      </c>
     </row>
     <row r="176" spans="2:22" ht="26.25">
       <c r="B176" t="s">
@@ -13698,6 +15309,15 @@
       <c r="V176" t="s">
         <v>1328</v>
       </c>
+      <c r="X176" t="s">
+        <v>353</v>
+      </c>
+      <c r="Y176" t="s">
+        <v>353</v>
+      </c>
+      <c r="Z176" t="s">
+        <v>353</v>
+      </c>
     </row>
     <row r="177" spans="2:22">
       <c r="B177" t="s">
@@ -13742,6 +15362,15 @@
       <c r="V177" t="s">
         <v>1329</v>
       </c>
+      <c r="X177" t="s">
+        <v>354</v>
+      </c>
+      <c r="Y177" t="s">
+        <v>354</v>
+      </c>
+      <c r="Z177" t="s">
+        <v>354</v>
+      </c>
     </row>
     <row r="178" spans="2:22">
       <c r="B178" t="s">
@@ -13786,6 +15415,15 @@
       <c r="V178" t="s">
         <v>1330</v>
       </c>
+      <c r="X178" t="s">
+        <v>355</v>
+      </c>
+      <c r="Y178" t="s">
+        <v>355</v>
+      </c>
+      <c r="Z178" t="s">
+        <v>355</v>
+      </c>
     </row>
     <row r="179" spans="2:22">
       <c r="B179" t="s">
@@ -13830,6 +15468,15 @@
       <c r="V179" t="s">
         <v>397</v>
       </c>
+      <c r="X179" t="s">
+        <v>397</v>
+      </c>
+      <c r="Y179" t="s">
+        <v>397</v>
+      </c>
+      <c r="Z179" t="s">
+        <v>397</v>
+      </c>
     </row>
     <row r="180" spans="2:22">
       <c r="B180" t="s">
@@ -13871,6 +15518,15 @@
       <c r="V180" t="s">
         <v>392</v>
       </c>
+      <c r="X180" t="s">
+        <v>392</v>
+      </c>
+      <c r="Y180" t="s">
+        <v>392</v>
+      </c>
+      <c r="Z180" t="s">
+        <v>392</v>
+      </c>
     </row>
     <row r="181" spans="2:22">
       <c r="B181" t="s">
@@ -13912,6 +15568,15 @@
       <c r="V181" t="s">
         <v>393</v>
       </c>
+      <c r="X181" t="s">
+        <v>393</v>
+      </c>
+      <c r="Y181" t="s">
+        <v>393</v>
+      </c>
+      <c r="Z181" t="s">
+        <v>393</v>
+      </c>
     </row>
     <row r="182" spans="2:22">
       <c r="B182" t="s">
@@ -13953,6 +15618,15 @@
       <c r="V182" t="s">
         <v>394</v>
       </c>
+      <c r="X182" t="s">
+        <v>394</v>
+      </c>
+      <c r="Y182" t="s">
+        <v>394</v>
+      </c>
+      <c r="Z182" t="s">
+        <v>394</v>
+      </c>
     </row>
     <row r="183" spans="2:22">
       <c r="B183" t="s">
@@ -13994,6 +15668,15 @@
       <c r="V183" t="s">
         <v>395</v>
       </c>
+      <c r="X183" t="s">
+        <v>395</v>
+      </c>
+      <c r="Y183" t="s">
+        <v>395</v>
+      </c>
+      <c r="Z183" t="s">
+        <v>395</v>
+      </c>
     </row>
     <row r="184" spans="2:22">
       <c r="B184" t="s">
@@ -14038,6 +15721,15 @@
       <c r="V184" t="s">
         <v>1331</v>
       </c>
+      <c r="X184" t="s">
+        <v>398</v>
+      </c>
+      <c r="Y184" t="s">
+        <v>398</v>
+      </c>
+      <c r="Z184" t="s">
+        <v>398</v>
+      </c>
     </row>
     <row r="185" spans="2:22">
       <c r="B185" t="s">
@@ -14082,6 +15774,15 @@
       <c r="V185" t="s">
         <v>1332</v>
       </c>
+      <c r="X185" t="s">
+        <v>399</v>
+      </c>
+      <c r="Y185" t="s">
+        <v>399</v>
+      </c>
+      <c r="Z185" t="s">
+        <v>399</v>
+      </c>
     </row>
     <row r="186" spans="2:22" ht="26.25">
       <c r="B186" t="s">
@@ -14126,6 +15827,15 @@
       <c r="V186" t="s">
         <v>1333</v>
       </c>
+      <c r="X186" t="s">
+        <v>400</v>
+      </c>
+      <c r="Y186" t="s">
+        <v>400</v>
+      </c>
+      <c r="Z186" t="s">
+        <v>400</v>
+      </c>
     </row>
     <row r="187" spans="2:22">
       <c r="B187" t="s">
@@ -14179,6 +15889,15 @@
       <c r="V187" t="s">
         <v>1267</v>
       </c>
+      <c r="X187" t="s">
+        <v>68</v>
+      </c>
+      <c r="Y187" t="s">
+        <v>68</v>
+      </c>
+      <c r="Z187" t="s">
+        <v>68</v>
+      </c>
     </row>
     <row r="188" spans="2:22">
       <c r="B188" t="s">
@@ -14223,6 +15942,15 @@
       <c r="V188" t="s">
         <v>1334</v>
       </c>
+      <c r="X188" t="s">
+        <v>365</v>
+      </c>
+      <c r="Y188" t="s">
+        <v>365</v>
+      </c>
+      <c r="Z188" t="s">
+        <v>365</v>
+      </c>
     </row>
     <row r="189" spans="2:22" ht="26.25">
       <c r="B189" t="s">
@@ -14267,6 +15995,15 @@
       <c r="V189" t="s">
         <v>1335</v>
       </c>
+      <c r="X189" t="s">
+        <v>401</v>
+      </c>
+      <c r="Y189" t="s">
+        <v>401</v>
+      </c>
+      <c r="Z189" t="s">
+        <v>401</v>
+      </c>
     </row>
     <row r="190" spans="2:22">
       <c r="B190" t="s">
@@ -14311,6 +16048,15 @@
       <c r="V190" t="s">
         <v>1336</v>
       </c>
+      <c r="X190" t="s">
+        <v>402</v>
+      </c>
+      <c r="Y190" t="s">
+        <v>402</v>
+      </c>
+      <c r="Z190" t="s">
+        <v>402</v>
+      </c>
     </row>
     <row r="191" spans="2:22" ht="39">
       <c r="B191" t="s">
@@ -14355,6 +16101,15 @@
       <c r="V191" t="s">
         <v>1337</v>
       </c>
+      <c r="X191" t="s">
+        <v>403</v>
+      </c>
+      <c r="Y191" t="s">
+        <v>403</v>
+      </c>
+      <c r="Z191" t="s">
+        <v>403</v>
+      </c>
     </row>
     <row r="192" spans="2:22">
       <c r="B192" t="s">
@@ -14399,6 +16154,15 @@
       <c r="V192" t="s">
         <v>1338</v>
       </c>
+      <c r="X192" t="s">
+        <v>405</v>
+      </c>
+      <c r="Y192" t="s">
+        <v>405</v>
+      </c>
+      <c r="Z192" t="s">
+        <v>405</v>
+      </c>
     </row>
     <row r="193" spans="2:22">
       <c r="B193" t="s">
@@ -14443,6 +16207,15 @@
       <c r="V193" t="s">
         <v>1339</v>
       </c>
+      <c r="X193" t="s">
+        <v>406</v>
+      </c>
+      <c r="Y193" t="s">
+        <v>406</v>
+      </c>
+      <c r="Z193" t="s">
+        <v>406</v>
+      </c>
     </row>
     <row r="194" spans="2:22">
       <c r="B194" t="s">
@@ -14487,6 +16260,15 @@
       <c r="V194" t="s">
         <v>1340</v>
       </c>
+      <c r="X194" t="s">
+        <v>408</v>
+      </c>
+      <c r="Y194" t="s">
+        <v>408</v>
+      </c>
+      <c r="Z194" t="s">
+        <v>408</v>
+      </c>
     </row>
     <row r="195" spans="2:22" ht="26.25">
       <c r="B195" t="s">
@@ -14528,6 +16310,15 @@
       <c r="V195" t="s">
         <v>1341</v>
       </c>
+      <c r="X195" t="s">
+        <v>410</v>
+      </c>
+      <c r="Y195" t="s">
+        <v>410</v>
+      </c>
+      <c r="Z195" t="s">
+        <v>410</v>
+      </c>
     </row>
     <row r="196" spans="2:22">
       <c r="B196" t="s">
@@ -14572,6 +16363,15 @@
       <c r="V196" t="s">
         <v>1342</v>
       </c>
+      <c r="X196" t="s">
+        <v>416</v>
+      </c>
+      <c r="Y196" t="s">
+        <v>416</v>
+      </c>
+      <c r="Z196" t="s">
+        <v>416</v>
+      </c>
     </row>
     <row r="197" spans="2:22">
       <c r="B197" t="s">
@@ -14616,6 +16416,15 @@
       <c r="V197" t="s">
         <v>1343</v>
       </c>
+      <c r="X197" t="s">
+        <v>414</v>
+      </c>
+      <c r="Y197" t="s">
+        <v>414</v>
+      </c>
+      <c r="Z197" t="s">
+        <v>414</v>
+      </c>
     </row>
     <row r="198" spans="2:22" ht="26.25">
       <c r="B198" t="s">
@@ -14660,6 +16469,15 @@
       <c r="V198" t="s">
         <v>1344</v>
       </c>
+      <c r="X198" t="s">
+        <v>1012</v>
+      </c>
+      <c r="Y198" t="s">
+        <v>1012</v>
+      </c>
+      <c r="Z198" t="s">
+        <v>1012</v>
+      </c>
     </row>
     <row r="199" spans="2:22">
       <c r="B199" t="s">
@@ -14701,6 +16519,15 @@
       <c r="V199" t="s">
         <v>890</v>
       </c>
+      <c r="X199" t="s">
+        <v>890</v>
+      </c>
+      <c r="Y199" t="s">
+        <v>890</v>
+      </c>
+      <c r="Z199" t="s">
+        <v>890</v>
+      </c>
     </row>
     <row r="200" spans="2:22">
       <c r="B200" t="s">
@@ -14742,6 +16569,15 @@
       <c r="V200" t="s">
         <v>1025</v>
       </c>
+      <c r="X200" t="s">
+        <v>907</v>
+      </c>
+      <c r="Y200" t="s">
+        <v>907</v>
+      </c>
+      <c r="Z200" t="s">
+        <v>907</v>
+      </c>
     </row>
     <row r="201" spans="2:22">
       <c r="B201" t="s">
@@ -14783,6 +16619,15 @@
       <c r="V201" t="s">
         <v>1025</v>
       </c>
+      <c r="X201" t="s">
+        <v>909</v>
+      </c>
+      <c r="Y201" t="s">
+        <v>909</v>
+      </c>
+      <c r="Z201" t="s">
+        <v>909</v>
+      </c>
     </row>
     <row r="202" spans="2:22">
       <c r="B202" t="s">
@@ -14824,6 +16669,15 @@
       <c r="V202" t="s">
         <v>43</v>
       </c>
+      <c r="X202" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y202" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z202" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="203" spans="2:22">
       <c r="B203" t="s">
@@ -14865,6 +16719,15 @@
       <c r="V203" t="s">
         <v>916</v>
       </c>
+      <c r="X203" t="s">
+        <v>911</v>
+      </c>
+      <c r="Y203" t="s">
+        <v>911</v>
+      </c>
+      <c r="Z203" t="s">
+        <v>911</v>
+      </c>
     </row>
     <row r="204" spans="2:22">
       <c r="B204" t="s">
@@ -14906,6 +16769,15 @@
       <c r="V204" t="s">
         <v>1025</v>
       </c>
+      <c r="X204" t="s">
+        <v>241</v>
+      </c>
+      <c r="Y204" t="s">
+        <v>241</v>
+      </c>
+      <c r="Z204" t="s">
+        <v>241</v>
+      </c>
     </row>
     <row r="205" spans="2:22">
       <c r="B205" t="s">
@@ -14950,6 +16822,15 @@
       <c r="V205" t="s">
         <v>1345</v>
       </c>
+      <c r="X205" t="s">
+        <v>1177</v>
+      </c>
+      <c r="Y205" t="s">
+        <v>1177</v>
+      </c>
+      <c r="Z205" t="s">
+        <v>1177</v>
+      </c>
     </row>
     <row r="206" spans="2:22">
       <c r="B206" t="s">
@@ -14994,6 +16875,15 @@
       <c r="V206" t="s">
         <v>916</v>
       </c>
+      <c r="X206" t="s">
+        <v>916</v>
+      </c>
+      <c r="Y206" t="s">
+        <v>916</v>
+      </c>
+      <c r="Z206" t="s">
+        <v>916</v>
+      </c>
     </row>
     <row r="207" spans="2:22">
       <c r="B207" t="s">
@@ -15038,6 +16928,15 @@
       <c r="V207" t="s">
         <v>1346</v>
       </c>
+      <c r="X207" t="s">
+        <v>923</v>
+      </c>
+      <c r="Y207" t="s">
+        <v>923</v>
+      </c>
+      <c r="Z207" t="s">
+        <v>923</v>
+      </c>
     </row>
     <row r="208" spans="2:22">
       <c r="B208" t="s">
@@ -15082,6 +16981,15 @@
       <c r="V208" t="s">
         <v>1347</v>
       </c>
+      <c r="X208" t="s">
+        <v>925</v>
+      </c>
+      <c r="Y208" t="s">
+        <v>925</v>
+      </c>
+      <c r="Z208" t="s">
+        <v>925</v>
+      </c>
     </row>
     <row r="209" spans="2:22">
       <c r="B209" t="s">
@@ -15123,6 +17031,15 @@
       <c r="V209" t="s">
         <v>43</v>
       </c>
+      <c r="X209" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y209" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z209" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="210" spans="2:22">
       <c r="B210" t="s">
@@ -15167,6 +17084,15 @@
       <c r="V210" t="s">
         <v>43</v>
       </c>
+      <c r="X210" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y210" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z210" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="211" spans="2:22">
       <c r="B211" t="s">
@@ -15211,6 +17137,15 @@
       <c r="V211" t="s">
         <v>1348</v>
       </c>
+      <c r="X211" t="s">
+        <v>206</v>
+      </c>
+      <c r="Y211" t="s">
+        <v>206</v>
+      </c>
+      <c r="Z211" t="s">
+        <v>206</v>
+      </c>
     </row>
     <row r="212" spans="2:22">
       <c r="B212" t="s">
@@ -15255,6 +17190,15 @@
       <c r="V212" t="s">
         <v>1349</v>
       </c>
+      <c r="X212" t="s">
+        <v>1091</v>
+      </c>
+      <c r="Y212" t="s">
+        <v>1091</v>
+      </c>
+      <c r="Z212" t="s">
+        <v>1091</v>
+      </c>
     </row>
     <row r="213" spans="2:22">
       <c r="B213" t="s">
@@ -15308,6 +17252,15 @@
       <c r="V213" t="s">
         <v>1350</v>
       </c>
+      <c r="X213" t="s">
+        <v>1092</v>
+      </c>
+      <c r="Y213" t="s">
+        <v>1092</v>
+      </c>
+      <c r="Z213" t="s">
+        <v>1092</v>
+      </c>
     </row>
     <row r="214" spans="2:22">
       <c r="B214" t="s">
@@ -15352,6 +17305,15 @@
       <c r="V214" t="s">
         <v>1351</v>
       </c>
+      <c r="X214" t="s">
+        <v>1056</v>
+      </c>
+      <c r="Y214" t="s">
+        <v>1056</v>
+      </c>
+      <c r="Z214" t="s">
+        <v>1056</v>
+      </c>
     </row>
     <row r="215" spans="2:22">
       <c r="B215" t="s">
@@ -15396,6 +17358,15 @@
       <c r="V215" t="s">
         <v>1085</v>
       </c>
+      <c r="X215" t="s">
+        <v>1085</v>
+      </c>
+      <c r="Y215" t="s">
+        <v>1085</v>
+      </c>
+      <c r="Z215" t="s">
+        <v>1085</v>
+      </c>
     </row>
     <row r="216" spans="2:22">
       <c r="B216" t="s">
@@ -15440,6 +17411,15 @@
       <c r="V216" t="s">
         <v>1054</v>
       </c>
+      <c r="X216" t="s">
+        <v>1054</v>
+      </c>
+      <c r="Y216" t="s">
+        <v>1054</v>
+      </c>
+      <c r="Z216" t="s">
+        <v>1054</v>
+      </c>
     </row>
     <row r="217" spans="2:22">
       <c r="B217" t="s">
@@ -15484,6 +17464,15 @@
       <c r="V217" t="s">
         <v>1352</v>
       </c>
+      <c r="X217" t="s">
+        <v>1059</v>
+      </c>
+      <c r="Y217" t="s">
+        <v>1059</v>
+      </c>
+      <c r="Z217" t="s">
+        <v>1059</v>
+      </c>
     </row>
     <row r="218" spans="2:22">
       <c r="B218" t="s">
@@ -15528,6 +17517,15 @@
       <c r="V218" t="s">
         <v>1353</v>
       </c>
+      <c r="X218" t="s">
+        <v>1066</v>
+      </c>
+      <c r="Y218" t="s">
+        <v>1066</v>
+      </c>
+      <c r="Z218" t="s">
+        <v>1066</v>
+      </c>
     </row>
     <row r="219" spans="2:22" ht="26.25">
       <c r="B219" t="s">
@@ -15572,6 +17570,15 @@
       <c r="V219" t="s">
         <v>1354</v>
       </c>
+      <c r="X219" t="s">
+        <v>1142</v>
+      </c>
+      <c r="Y219" t="s">
+        <v>1142</v>
+      </c>
+      <c r="Z219" t="s">
+        <v>1142</v>
+      </c>
     </row>
     <row r="220" spans="2:22">
       <c r="B220" t="s">
@@ -15613,6 +17620,15 @@
       <c r="V220" t="s">
         <v>1025</v>
       </c>
+      <c r="X220" t="s">
+        <v>1116</v>
+      </c>
+      <c r="Y220" t="s">
+        <v>1116</v>
+      </c>
+      <c r="Z220" t="s">
+        <v>1116</v>
+      </c>
     </row>
     <row r="221" spans="2:22">
       <c r="B221" t="s">
@@ -15654,6 +17670,15 @@
       <c r="V221" t="s">
         <v>1025</v>
       </c>
+      <c r="X221" t="s">
+        <v>1130</v>
+      </c>
+      <c r="Y221" t="s">
+        <v>1130</v>
+      </c>
+      <c r="Z221" t="s">
+        <v>1130</v>
+      </c>
     </row>
     <row r="222" spans="2:22">
       <c r="B222" t="s">
@@ -15695,6 +17720,15 @@
       <c r="V222" t="s">
         <v>1025</v>
       </c>
+      <c r="X222" t="s">
+        <v>1131</v>
+      </c>
+      <c r="Y222" t="s">
+        <v>1131</v>
+      </c>
+      <c r="Z222" t="s">
+        <v>1131</v>
+      </c>
     </row>
     <row r="223" spans="2:22">
       <c r="B223" t="s">
@@ -15736,6 +17770,15 @@
       <c r="V223" t="s">
         <v>1025</v>
       </c>
+      <c r="X223" t="s">
+        <v>916</v>
+      </c>
+      <c r="Y223" t="s">
+        <v>916</v>
+      </c>
+      <c r="Z223" t="s">
+        <v>916</v>
+      </c>
     </row>
     <row r="224" spans="2:22">
       <c r="B224" t="s">
@@ -15777,6 +17820,15 @@
       <c r="V224" t="s">
         <v>1025</v>
       </c>
+      <c r="X224" t="s">
+        <v>1140</v>
+      </c>
+      <c r="Y224" t="s">
+        <v>1140</v>
+      </c>
+      <c r="Z224" t="s">
+        <v>1140</v>
+      </c>
     </row>
     <row r="225" spans="2:22">
       <c r="B225" t="s">
@@ -15818,6 +17870,15 @@
       <c r="V225" t="s">
         <v>1025</v>
       </c>
+      <c r="X225" t="s">
+        <v>1128</v>
+      </c>
+      <c r="Y225" t="s">
+        <v>1128</v>
+      </c>
+      <c r="Z225" t="s">
+        <v>1128</v>
+      </c>
     </row>
     <row r="226" spans="2:22">
       <c r="B226" t="s">
@@ -15859,6 +17920,15 @@
       <c r="V226" t="s">
         <v>1025</v>
       </c>
+      <c r="X226" t="s">
+        <v>1132</v>
+      </c>
+      <c r="Y226" t="s">
+        <v>1132</v>
+      </c>
+      <c r="Z226" t="s">
+        <v>1132</v>
+      </c>
     </row>
     <row r="227" spans="2:22">
       <c r="B227" t="s">
@@ -15900,6 +17970,15 @@
       <c r="V227" t="s">
         <v>1025</v>
       </c>
+      <c r="X227" t="s">
+        <v>1133</v>
+      </c>
+      <c r="Y227" t="s">
+        <v>1133</v>
+      </c>
+      <c r="Z227" t="s">
+        <v>1133</v>
+      </c>
     </row>
     <row r="228" spans="2:22">
       <c r="B228" t="s">
@@ -15941,6 +18020,15 @@
       <c r="V228" t="s">
         <v>1025</v>
       </c>
+      <c r="X228" t="s">
+        <v>1129</v>
+      </c>
+      <c r="Y228" t="s">
+        <v>1129</v>
+      </c>
+      <c r="Z228" t="s">
+        <v>1129</v>
+      </c>
     </row>
     <row r="229" spans="2:22">
       <c r="B229" t="s">
@@ -15982,6 +18070,15 @@
       <c r="V229" t="s">
         <v>1025</v>
       </c>
+      <c r="X229" t="s">
+        <v>1134</v>
+      </c>
+      <c r="Y229" t="s">
+        <v>1134</v>
+      </c>
+      <c r="Z229" t="s">
+        <v>1134</v>
+      </c>
     </row>
     <row r="230" spans="2:22">
       <c r="B230" t="s">
@@ -16023,6 +18120,15 @@
       <c r="V230" t="s">
         <v>1025</v>
       </c>
+      <c r="X230" t="s">
+        <v>1135</v>
+      </c>
+      <c r="Y230" t="s">
+        <v>1135</v>
+      </c>
+      <c r="Z230" t="s">
+        <v>1135</v>
+      </c>
     </row>
     <row r="231" spans="2:22">
       <c r="B231" t="s">
@@ -16064,6 +18170,15 @@
       <c r="V231" t="s">
         <v>1025</v>
       </c>
+      <c r="X231" t="s">
+        <v>1141</v>
+      </c>
+      <c r="Y231" t="s">
+        <v>1141</v>
+      </c>
+      <c r="Z231" t="s">
+        <v>1141</v>
+      </c>
     </row>
     <row r="232" spans="2:22">
       <c r="B232" t="s">
@@ -16105,6 +18220,15 @@
       <c r="V232" t="s">
         <v>1025</v>
       </c>
+      <c r="X232" t="s">
+        <v>1138</v>
+      </c>
+      <c r="Y232" t="s">
+        <v>1138</v>
+      </c>
+      <c r="Z232" t="s">
+        <v>1138</v>
+      </c>
     </row>
     <row r="233" spans="2:22">
       <c r="B233" t="s">
@@ -16146,6 +18270,15 @@
       <c r="V233" t="s">
         <v>43</v>
       </c>
+      <c r="X233" t="s">
+        <v>43</v>
+      </c>
+      <c r="Y233" t="s">
+        <v>43</v>
+      </c>
+      <c r="Z233" t="s">
+        <v>43</v>
+      </c>
     </row>
     <row r="234" spans="2:22">
       <c r="B234" t="s">
@@ -16187,6 +18320,15 @@
       <c r="V234" t="s">
         <v>1025</v>
       </c>
+      <c r="X234" t="s">
+        <v>1155</v>
+      </c>
+      <c r="Y234" t="s">
+        <v>1155</v>
+      </c>
+      <c r="Z234" t="s">
+        <v>1155</v>
+      </c>
     </row>
     <row r="235" spans="2:22" ht="26.25">
       <c r="B235" t="s">
@@ -16231,6 +18373,15 @@
       <c r="V235" t="s">
         <v>1355</v>
       </c>
+      <c r="X235" t="s">
+        <v>1152</v>
+      </c>
+      <c r="Y235" t="s">
+        <v>1152</v>
+      </c>
+      <c r="Z235" t="s">
+        <v>1152</v>
+      </c>
     </row>
     <row r="236" spans="2:22">
       <c r="B236" t="s">
@@ -16272,6 +18423,15 @@
       <c r="V236" t="s">
         <v>1025</v>
       </c>
+      <c r="X236" t="s">
+        <v>1154</v>
+      </c>
+      <c r="Y236" t="s">
+        <v>1154</v>
+      </c>
+      <c r="Z236" t="s">
+        <v>1154</v>
+      </c>
     </row>
     <row r="237" spans="2:22">
       <c r="B237" t="s">
@@ -16313,6 +18473,15 @@
       <c r="V237" t="s">
         <v>43</v>
       </c>
+      <c r="X237" t="s">
+        <v>1157</v>
+      </c>
+      <c r="Y237" t="s">
+        <v>1157</v>
+      </c>
+      <c r="Z237" t="s">
+        <v>1157</v>
+      </c>
     </row>
     <row r="238" spans="2:22">
       <c r="B238" t="s">
@@ -16357,6 +18526,15 @@
       <c r="V238" t="s">
         <v>1159</v>
       </c>
+      <c r="X238" t="s">
+        <v>1159</v>
+      </c>
+      <c r="Y238" t="s">
+        <v>1159</v>
+      </c>
+      <c r="Z238" t="s">
+        <v>1159</v>
+      </c>
     </row>
     <row r="239" spans="2:22">
       <c r="B239" t="s">
@@ -16401,6 +18579,15 @@
       <c r="V239" t="s">
         <v>1356</v>
       </c>
+      <c r="X239" t="s">
+        <v>1029</v>
+      </c>
+      <c r="Y239" t="s">
+        <v>1029</v>
+      </c>
+      <c r="Z239" t="s">
+        <v>1029</v>
+      </c>
     </row>
     <row r="240" spans="2:22">
       <c r="B240" t="s">
@@ -16445,6 +18632,15 @@
       <c r="V240" t="s">
         <v>1357</v>
       </c>
+      <c r="X240" t="s">
+        <v>1161</v>
+      </c>
+      <c r="Y240" t="s">
+        <v>1161</v>
+      </c>
+      <c r="Z240" t="s">
+        <v>1161</v>
+      </c>
     </row>
     <row r="241" spans="2:22">
       <c r="B241" t="s">
@@ -16486,6 +18682,15 @@
       <c r="V241" t="s">
         <v>1162</v>
       </c>
+      <c r="X241" t="s">
+        <v>1162</v>
+      </c>
+      <c r="Y241" t="s">
+        <v>1162</v>
+      </c>
+      <c r="Z241" t="s">
+        <v>1162</v>
+      </c>
     </row>
     <row r="242" spans="2:22">
       <c r="B242" t="s">
@@ -16527,6 +18732,15 @@
       <c r="V242" t="s">
         <v>1236</v>
       </c>
+      <c r="X242" t="s">
+        <v>1163</v>
+      </c>
+      <c r="Y242" t="s">
+        <v>1163</v>
+      </c>
+      <c r="Z242" t="s">
+        <v>1163</v>
+      </c>
     </row>
     <row r="243" spans="2:22">
       <c r="B243" t="s">
@@ -16568,6 +18782,15 @@
       <c r="V243" t="s">
         <v>1164</v>
       </c>
+      <c r="X243" t="s">
+        <v>1164</v>
+      </c>
+      <c r="Y243" t="s">
+        <v>1164</v>
+      </c>
+      <c r="Z243" t="s">
+        <v>1164</v>
+      </c>
     </row>
     <row r="244" spans="2:22">
       <c r="B244" t="s">
@@ -16612,6 +18835,15 @@
       <c r="V244" t="s">
         <v>1356</v>
       </c>
+      <c r="X244" t="s">
+        <v>1029</v>
+      </c>
+      <c r="Y244" t="s">
+        <v>1029</v>
+      </c>
+      <c r="Z244" t="s">
+        <v>1029</v>
+      </c>
     </row>
     <row r="245" spans="2:22">
       <c r="B245" t="s">
@@ -16656,6 +18888,15 @@
       <c r="V245" t="s">
         <v>1358</v>
       </c>
+      <c r="X245" t="s">
+        <v>1168</v>
+      </c>
+      <c r="Y245" t="s">
+        <v>1168</v>
+      </c>
+      <c r="Z245" t="s">
+        <v>1168</v>
+      </c>
     </row>
     <row r="246" spans="2:22">
       <c r="B246" t="s">
@@ -16700,6 +18941,15 @@
       <c r="V246" t="s">
         <v>1359</v>
       </c>
+      <c r="X246" t="s">
+        <v>1169</v>
+      </c>
+      <c r="Y246" t="s">
+        <v>1169</v>
+      </c>
+      <c r="Z246" t="s">
+        <v>1169</v>
+      </c>
     </row>
     <row r="247" spans="2:22">
       <c r="B247" t="s">
@@ -16741,6 +18991,15 @@
       <c r="V247" t="s">
         <v>1176</v>
       </c>
+      <c r="X247" t="s">
+        <v>1176</v>
+      </c>
+      <c r="Y247" t="s">
+        <v>1176</v>
+      </c>
+      <c r="Z247" t="s">
+        <v>1176</v>
+      </c>
     </row>
     <row r="248" spans="2:22">
       <c r="B248" t="s">
@@ -16782,6 +19041,15 @@
       <c r="V248" t="s">
         <v>1179</v>
       </c>
+      <c r="X248" t="s">
+        <v>1179</v>
+      </c>
+      <c r="Y248" t="s">
+        <v>1179</v>
+      </c>
+      <c r="Z248" t="s">
+        <v>1179</v>
+      </c>
     </row>
     <row r="249" spans="2:22">
       <c r="B249" t="s">
@@ -16823,6 +19091,15 @@
       <c r="V249" t="s">
         <v>1179</v>
       </c>
+      <c r="X249" t="s">
+        <v>1179</v>
+      </c>
+      <c r="Y249" t="s">
+        <v>1179</v>
+      </c>
+      <c r="Z249" t="s">
+        <v>1179</v>
+      </c>
     </row>
     <row r="250" spans="2:22">
       <c r="B250" t="s">
@@ -16867,6 +19144,15 @@
       <c r="V250" t="s">
         <v>1360</v>
       </c>
+      <c r="X250" t="s">
+        <v>1182</v>
+      </c>
+      <c r="Y250" t="s">
+        <v>1182</v>
+      </c>
+      <c r="Z250" t="s">
+        <v>1182</v>
+      </c>
     </row>
     <row r="251" spans="2:22">
       <c r="B251" t="s">
@@ -16911,6 +19197,15 @@
       <c r="V251" t="s">
         <v>1361</v>
       </c>
+      <c r="X251" t="s">
+        <v>1191</v>
+      </c>
+      <c r="Y251" t="s">
+        <v>1191</v>
+      </c>
+      <c r="Z251" t="s">
+        <v>1191</v>
+      </c>
     </row>
     <row r="252" spans="2:22">
       <c r="B252" t="s">
@@ -16955,6 +19250,15 @@
       <c r="V252" t="s">
         <v>1362</v>
       </c>
+      <c r="X252" t="s">
+        <v>1192</v>
+      </c>
+      <c r="Y252" t="s">
+        <v>1192</v>
+      </c>
+      <c r="Z252" t="s">
+        <v>1192</v>
+      </c>
     </row>
     <row r="253" spans="2:22" ht="26.25">
       <c r="B253" t="s">
@@ -16999,6 +19303,15 @@
       <c r="V253" t="s">
         <v>1363</v>
       </c>
+      <c r="X253" t="s">
+        <v>1207</v>
+      </c>
+      <c r="Y253" t="s">
+        <v>1207</v>
+      </c>
+      <c r="Z253" t="s">
+        <v>1207</v>
+      </c>
     </row>
     <row r="254" spans="2:22">
       <c r="B254" t="s">
@@ -17040,6 +19353,15 @@
       <c r="V254" t="s">
         <v>1025</v>
       </c>
+      <c r="X254" t="s">
+        <v>1253</v>
+      </c>
+      <c r="Y254" t="s">
+        <v>1253</v>
+      </c>
+      <c r="Z254" t="s">
+        <v>1253</v>
+      </c>
     </row>
     <row r="255" spans="2:22">
       <c r="B255" t="s">
@@ -17081,6 +19403,15 @@
       <c r="V255" t="s">
         <v>1025</v>
       </c>
+      <c r="X255" t="s">
+        <v>1256</v>
+      </c>
+      <c r="Y255" t="s">
+        <v>1256</v>
+      </c>
+      <c r="Z255" t="s">
+        <v>1256</v>
+      </c>
     </row>
     <row r="256">
       <c r="B256" t="s">
@@ -17122,6 +19453,15 @@
       <c r="V256" t="s">
         <v>1368</v>
       </c>
+      <c r="X256" t="s">
+        <v>1368</v>
+      </c>
+      <c r="Y256" t="s">
+        <v>1368</v>
+      </c>
+      <c r="Z256" t="s">
+        <v>1368</v>
+      </c>
     </row>
     <row r="257">
       <c r="B257" t="s">
@@ -17163,6 +19503,15 @@
       <c r="V257" t="s">
         <v>1370</v>
       </c>
+      <c r="X257" t="s">
+        <v>238</v>
+      </c>
+      <c r="Y257" t="s">
+        <v>238</v>
+      </c>
+      <c r="Z257" t="s">
+        <v>238</v>
+      </c>
     </row>
     <row r="258">
       <c r="B258" t="s">
@@ -17178,7 +19527,7 @@
         <v>41</v>
       </c>
       <c r="F258" t="s">
-        <v>1383</v>
+        <v>1373</v>
       </c>
       <c r="G258" t="s">
         <v>1370</v>
@@ -17203,6 +19552,15 @@
       </c>
       <c r="V258" t="s">
         <v>1370</v>
+      </c>
+      <c r="X258" t="s">
+        <v>1373</v>
+      </c>
+      <c r="Y258" t="s">
+        <v>1373</v>
+      </c>
+      <c r="Z258" t="s">
+        <v>1373</v>
       </c>
     </row>
     <row r="259">
@@ -17219,7 +19577,7 @@
         <v>41</v>
       </c>
       <c r="F259" t="s">
-        <v>1384</v>
+        <v>1374</v>
       </c>
       <c r="G259" t="s">
         <v>1370</v>
@@ -17244,6 +19602,165 @@
       </c>
       <c r="V259" t="s">
         <v>1370</v>
+      </c>
+      <c r="X259" t="s">
+        <v>1374</v>
+      </c>
+      <c r="Y259" t="s">
+        <v>1374</v>
+      </c>
+      <c r="Z259" t="s">
+        <v>1374</v>
+      </c>
+    </row>
+    <row r="260">
+      <c r="B260" t="s">
+        <v>1388</v>
+      </c>
+      <c r="C260" t="s">
+        <v>37</v>
+      </c>
+      <c r="D260" t="s">
+        <v>40</v>
+      </c>
+      <c r="E260" t="s">
+        <v>41</v>
+      </c>
+      <c r="F260" t="s">
+        <v>1389</v>
+      </c>
+      <c r="G260" t="s">
+        <v>1389</v>
+      </c>
+      <c r="I260" t="s">
+        <v>1389</v>
+      </c>
+      <c r="J260" t="s">
+        <v>1389</v>
+      </c>
+      <c r="K260" t="s">
+        <v>1389</v>
+      </c>
+      <c r="L260" t="s">
+        <v>1389</v>
+      </c>
+      <c r="M260" t="s">
+        <v>1389</v>
+      </c>
+      <c r="N260" t="s">
+        <v>1389</v>
+      </c>
+      <c r="V260" t="s">
+        <v>1389</v>
+      </c>
+      <c r="X260" t="s">
+        <v>1389</v>
+      </c>
+      <c r="Y260" t="s">
+        <v>1389</v>
+      </c>
+      <c r="Z260" t="s">
+        <v>1389</v>
+      </c>
+    </row>
+    <row r="261">
+      <c r="B261" t="s">
+        <v>1390</v>
+      </c>
+      <c r="C261" t="s">
+        <v>37</v>
+      </c>
+      <c r="D261" t="s">
+        <v>40</v>
+      </c>
+      <c r="E261" t="s">
+        <v>41</v>
+      </c>
+      <c r="F261" t="s">
+        <v>1391</v>
+      </c>
+      <c r="G261" t="s">
+        <v>1391</v>
+      </c>
+      <c r="I261" t="s">
+        <v>1391</v>
+      </c>
+      <c r="J261" t="s">
+        <v>1391</v>
+      </c>
+      <c r="K261" t="s">
+        <v>1391</v>
+      </c>
+      <c r="L261" t="s">
+        <v>1391</v>
+      </c>
+      <c r="M261" t="s">
+        <v>1391</v>
+      </c>
+      <c r="N261" t="s">
+        <v>1391</v>
+      </c>
+      <c r="V261" t="s">
+        <v>1391</v>
+      </c>
+      <c r="X261" t="s">
+        <v>1391</v>
+      </c>
+      <c r="Y261" t="s">
+        <v>1391</v>
+      </c>
+      <c r="Z261" t="s">
+        <v>1391</v>
+      </c>
+    </row>
+    <row r="262">
+      <c r="B262" t="s">
+        <v>1392</v>
+      </c>
+      <c r="C262" t="s">
+        <v>37</v>
+      </c>
+      <c r="D262" t="s">
+        <v>40</v>
+      </c>
+      <c r="E262" t="s">
+        <v>41</v>
+      </c>
+      <c r="F262" t="s">
+        <v>1393</v>
+      </c>
+      <c r="G262" t="s">
+        <v>1393</v>
+      </c>
+      <c r="I262" t="s">
+        <v>1393</v>
+      </c>
+      <c r="J262" t="s">
+        <v>1393</v>
+      </c>
+      <c r="K262" t="s">
+        <v>1393</v>
+      </c>
+      <c r="L262" t="s">
+        <v>1393</v>
+      </c>
+      <c r="M262" t="s">
+        <v>1393</v>
+      </c>
+      <c r="N262" t="s">
+        <v>1393</v>
+      </c>
+      <c r="V262" t="s">
+        <v>1393</v>
+      </c>
+      <c r="X262" t="s">
+        <v>1393</v>
+      </c>
+      <c r="Y262" t="s">
+        <v>1393</v>
+      </c>
+      <c r="Z262" t="s">
+        <v>1393</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Start implementing automatic drying
</commit_message>
<xml_diff>
--- a/RECOVER/assets/texts/texts.xlsx
+++ b/RECOVER/assets/texts/texts.xlsx
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="132838" uniqueCount="1397">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147778" uniqueCount="1398">
   <si>
     <t xml:space="preserve">Font</t>
   </si>
@@ -4455,6 +4455,10 @@
   </si>
   <si>
     <t xml:space="preserve">UA-TYPOGRAPHY</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Possible moisture detected - attempting to clear.
+Please wait...</t>
   </si>
 </sst>
 </file>
@@ -19465,7 +19469,7 @@
     </row>
     <row r="257">
       <c r="B257" t="s">
-        <v>1369</v>
+        <v>1372</v>
       </c>
       <c r="C257" t="s">
         <v>37</v>
@@ -19477,7 +19481,7 @@
         <v>41</v>
       </c>
       <c r="F257" t="s">
-        <v>238</v>
+        <v>1397</v>
       </c>
       <c r="G257" t="s">
         <v>1370</v>
@@ -19504,18 +19508,18 @@
         <v>1370</v>
       </c>
       <c r="X257" t="s">
-        <v>238</v>
+        <v>1374</v>
       </c>
       <c r="Y257" t="s">
-        <v>238</v>
+        <v>1374</v>
       </c>
       <c r="Z257" t="s">
-        <v>238</v>
+        <v>1374</v>
       </c>
     </row>
     <row r="258">
       <c r="B258" t="s">
-        <v>1371</v>
+        <v>1388</v>
       </c>
       <c r="C258" t="s">
         <v>37</v>
@@ -19527,45 +19531,45 @@
         <v>41</v>
       </c>
       <c r="F258" t="s">
-        <v>1373</v>
+        <v>1389</v>
       </c>
       <c r="G258" t="s">
-        <v>1370</v>
+        <v>1389</v>
       </c>
       <c r="I258" t="s">
-        <v>1370</v>
+        <v>1389</v>
       </c>
       <c r="J258" t="s">
-        <v>1370</v>
+        <v>1389</v>
       </c>
       <c r="K258" t="s">
-        <v>1370</v>
+        <v>1389</v>
       </c>
       <c r="L258" t="s">
-        <v>1370</v>
+        <v>1389</v>
       </c>
       <c r="M258" t="s">
-        <v>1370</v>
+        <v>1389</v>
       </c>
       <c r="N258" t="s">
-        <v>1370</v>
+        <v>1389</v>
       </c>
       <c r="V258" t="s">
-        <v>1370</v>
+        <v>1389</v>
       </c>
       <c r="X258" t="s">
-        <v>1373</v>
+        <v>1389</v>
       </c>
       <c r="Y258" t="s">
-        <v>1373</v>
+        <v>1389</v>
       </c>
       <c r="Z258" t="s">
-        <v>1373</v>
+        <v>1389</v>
       </c>
     </row>
     <row r="259">
       <c r="B259" t="s">
-        <v>1372</v>
+        <v>1390</v>
       </c>
       <c r="C259" t="s">
         <v>37</v>
@@ -19577,45 +19581,45 @@
         <v>41</v>
       </c>
       <c r="F259" t="s">
-        <v>1374</v>
+        <v>1391</v>
       </c>
       <c r="G259" t="s">
-        <v>1370</v>
+        <v>1391</v>
       </c>
       <c r="I259" t="s">
-        <v>1370</v>
+        <v>1391</v>
       </c>
       <c r="J259" t="s">
-        <v>1370</v>
+        <v>1391</v>
       </c>
       <c r="K259" t="s">
-        <v>1370</v>
+        <v>1391</v>
       </c>
       <c r="L259" t="s">
-        <v>1370</v>
+        <v>1391</v>
       </c>
       <c r="M259" t="s">
-        <v>1370</v>
+        <v>1391</v>
       </c>
       <c r="N259" t="s">
-        <v>1370</v>
+        <v>1391</v>
       </c>
       <c r="V259" t="s">
-        <v>1370</v>
+        <v>1391</v>
       </c>
       <c r="X259" t="s">
-        <v>1374</v>
+        <v>1391</v>
       </c>
       <c r="Y259" t="s">
-        <v>1374</v>
+        <v>1391</v>
       </c>
       <c r="Z259" t="s">
-        <v>1374</v>
+        <v>1391</v>
       </c>
     </row>
     <row r="260">
       <c r="B260" t="s">
-        <v>1388</v>
+        <v>1392</v>
       </c>
       <c r="C260" t="s">
         <v>37</v>
@@ -19627,142 +19631,44 @@
         <v>41</v>
       </c>
       <c r="F260" t="s">
-        <v>1389</v>
+        <v>1393</v>
       </c>
       <c r="G260" t="s">
-        <v>1389</v>
+        <v>1393</v>
       </c>
       <c r="I260" t="s">
-        <v>1389</v>
+        <v>1393</v>
       </c>
       <c r="J260" t="s">
-        <v>1389</v>
+        <v>1393</v>
       </c>
       <c r="K260" t="s">
-        <v>1389</v>
+        <v>1393</v>
       </c>
       <c r="L260" t="s">
-        <v>1389</v>
+        <v>1393</v>
       </c>
       <c r="M260" t="s">
-        <v>1389</v>
+        <v>1393</v>
       </c>
       <c r="N260" t="s">
-        <v>1389</v>
+        <v>1393</v>
       </c>
       <c r="V260" t="s">
-        <v>1389</v>
+        <v>1393</v>
       </c>
       <c r="X260" t="s">
-        <v>1389</v>
+        <v>1393</v>
       </c>
       <c r="Y260" t="s">
-        <v>1389</v>
+        <v>1393</v>
       </c>
       <c r="Z260" t="s">
-        <v>1389</v>
-      </c>
-    </row>
-    <row r="261">
-      <c r="B261" t="s">
-        <v>1390</v>
-      </c>
-      <c r="C261" t="s">
-        <v>37</v>
-      </c>
-      <c r="D261" t="s">
-        <v>40</v>
-      </c>
-      <c r="E261" t="s">
-        <v>41</v>
-      </c>
-      <c r="F261" t="s">
-        <v>1391</v>
-      </c>
-      <c r="G261" t="s">
-        <v>1391</v>
-      </c>
-      <c r="I261" t="s">
-        <v>1391</v>
-      </c>
-      <c r="J261" t="s">
-        <v>1391</v>
-      </c>
-      <c r="K261" t="s">
-        <v>1391</v>
-      </c>
-      <c r="L261" t="s">
-        <v>1391</v>
-      </c>
-      <c r="M261" t="s">
-        <v>1391</v>
-      </c>
-      <c r="N261" t="s">
-        <v>1391</v>
-      </c>
-      <c r="V261" t="s">
-        <v>1391</v>
-      </c>
-      <c r="X261" t="s">
-        <v>1391</v>
-      </c>
-      <c r="Y261" t="s">
-        <v>1391</v>
-      </c>
-      <c r="Z261" t="s">
-        <v>1391</v>
-      </c>
-    </row>
-    <row r="262">
-      <c r="B262" t="s">
-        <v>1392</v>
-      </c>
-      <c r="C262" t="s">
-        <v>37</v>
-      </c>
-      <c r="D262" t="s">
-        <v>40</v>
-      </c>
-      <c r="E262" t="s">
-        <v>41</v>
-      </c>
-      <c r="F262" t="s">
         <v>1393</v>
       </c>
-      <c r="G262" t="s">
-        <v>1393</v>
-      </c>
-      <c r="I262" t="s">
-        <v>1393</v>
-      </c>
-      <c r="J262" t="s">
-        <v>1393</v>
-      </c>
-      <c r="K262" t="s">
-        <v>1393</v>
-      </c>
-      <c r="L262" t="s">
-        <v>1393</v>
-      </c>
-      <c r="M262" t="s">
-        <v>1393</v>
-      </c>
-      <c r="N262" t="s">
-        <v>1393</v>
-      </c>
-      <c r="V262" t="s">
-        <v>1393</v>
-      </c>
-      <c r="X262" t="s">
-        <v>1393</v>
-      </c>
-      <c r="Y262" t="s">
-        <v>1393</v>
-      </c>
-      <c r="Z262" t="s">
-        <v>1393</v>
-      </c>
-    </row>
+    </row>
+    <row r="261"/>
+    <row r="262"/>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="B2:E2"/>

</xml_diff>